<commit_message>
added: algorithm that finds the respective columns of the model worksheet
</commit_message>
<xml_diff>
--- a/PropProAssistant/Models/LicitaNet/LN_01.xlsx
+++ b/PropProAssistant/Models/LicitaNet/LN_01.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
   <si>
     <t>LOTE</t>
   </si>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">ÁCIDO TRANEXÂMICO - PRINCÍPIO ATIVO: ÁCIDO TRANEXÊMICO; CONCENTRAÇÃO/DOSAGEM:  50MG/ML; FORMA FARMACÊUTICA: SOLUÇÃO INJETÁVEL; APRESENTAÇÃO: AMPOLAS 5ML.</t>
   </si>
   <si>
-    <t>HIPOLABOR</t>
+    <t/>
   </si>
   <si>
     <t>ADREN - PRINCÍPIO ATIVO: EPINEFRINA; CONCENTRAÇÃO/DOSAGEM: 1MG/ML; FORMA FARMACÊUTICA: SOLUÇÃO INJETÁVEL; APRESENTAÇÃO: AMPOLAS 1ML;</t>
@@ -58,9 +58,6 @@
     <t>ALBENDAZOL - PRINCIPIO ATIVO: ALBENDAZOL; CONCENTRACAO/DOSAGEM: 40 MG/ML; FORMA FARMACEUTICA: SUSPENSAO ORAL; APRESENTACAO: FRASCO 10ML.</t>
   </si>
   <si>
-    <t>GEOLAB</t>
-  </si>
-  <si>
     <t>AMINOFILINA - PRINCÍPIO ATIVO: AMINOFILINA; CONCENTRAÇÃO/DOSAGEM: 24MG/ML; FORMA FARMACÊUTICA: SOLUÇÃO INJETÁVEL; APRESENTAÇÃO: AMPOLAS 10ML</t>
   </si>
   <si>
@@ -70,66 +67,39 @@
     <t>AMOXICILINA - PRINCIPIO ATIVO: AMOXICILINA; CONCENTRACAO/DOSAGEM: 250 MG/5 ML; FORMA FARMACEUTICA: PO PARA SUSPENSAO ORAL; APRESENTACAO: FRASCO 60ML; COMPONENTE: COPO MEDIDOR;</t>
   </si>
   <si>
-    <t>GERMED</t>
-  </si>
-  <si>
     <t>AMOXICILINA + ASSOCIACOES - PRINCIPIO ATIVO: AMOXICILINA + CLAVULANATO DE POTASSIO; CONCENTRACAO/DOSAGEM: 50 MG/ML + 12,5 MG/ML; FORMA FARMACEUTICA: PO PARA SUSPENSAO ORAL; APRESENTACAO: FRASCO 75 ML; COMPONENTE: DOSADOR;</t>
   </si>
   <si>
-    <t>EMS</t>
-  </si>
-  <si>
     <t>AMOXICILINA + ASSOCIACOES - PRINCIPIO ATIVO: AMOXICILINA + CLAVULANATO DE POTASSIO; CONCENTRACAO/DOSAGEM: 500 MG + 125 MG; FORMA FARMACEUTICA: COMPRIMIDO REVESTIDO.</t>
   </si>
   <si>
     <t>ATENOLOL - PRINCIPIO ATIVO: ATENOLOL; CONCENTRACAO/DOSAGEM: 100 MG; FORMA FARMACEUTICA: COMPRIMIDO.</t>
   </si>
   <si>
-    <t>LEGRAND</t>
-  </si>
-  <si>
     <t>ATROPINA - PRINCIPIO ATIVO: ATROPINA, SULFATO; CONCENTRACAO/DOSAGEM: 0,25 MG/ML; FORMA FARMACEUTICA: SOLUCAO INJETAVEL; APRESENTACAO: AMPOLA 1 ML.</t>
   </si>
   <si>
-    <t>FARMACE</t>
-  </si>
-  <si>
     <t>AZITROMICINA - PRINCIPIO ATIVO: AZITROMICINA DI-HIDRATADA; CONCENTRACAO/DOSAGEM: 200 MG/5 ML; FORMA FARMACEUTICA: PO PARA SUSPENSAO ORAL; APRESENTACAO: FRASCO 15 ML; COMPONENTE: FRASCO DILUENTE + SERINGA DOSADORA;</t>
   </si>
   <si>
-    <t>PHARLAB</t>
-  </si>
-  <si>
     <t>BROMETO DE IPRATROPIO - PRINCIPIO ATIVO: IPRATROPIO, BROMETO; CONCENTRACAO/DOSAGEM: 0,25 MG/ML; FORMA FARMACEUTICA: SOLUCAO PARA INALACAO; APRESENTACAO: FRASCO 20 ML.</t>
   </si>
   <si>
-    <t>TEUTO</t>
-  </si>
-  <si>
     <t>BROMOPRIDA - PRINCÍPIO ATIVO: BROMOPRIDA; CONCENTRAÇÃO/DOSAGEM: 5MG/ML; FORMA FARMACÊUTICA: SOLUÇÃO INJETÁVEL; APRESENTAÇÃO: AMPOLAS 2ML</t>
   </si>
   <si>
     <t>CARVEDILOL - PRINCIPIO ATIVO: CARVEDILOL; CONCENTRACAO/DOSAGEM: 25 MG; FORMA FARMACEUTICA: COMPRIMIDO.</t>
   </si>
   <si>
-    <t>MULTILAB</t>
-  </si>
-  <si>
     <t>CEFALEXINA - PRINCIPIO ATIVO: CEFALEXINA; CONCENTRACAO/DOSAGEM: 500 MG; FORMA FARMACEUTICA: COMPRIMIDO REVESTIDO.</t>
   </si>
   <si>
     <t>CEFTRIAXONA - PRINCIPIO ATIVO: CEFTRIAXONA; CONCENTRACAO/DOSAGEM: 1000 MG; FORMA FARMACEUTICA: PO PARA SOLUCAO INJETAVEL; APRESENTACAO: FRASCO-AMPOLA;</t>
   </si>
   <si>
-    <t>BLAU</t>
-  </si>
-  <si>
     <t>CICLOBENZAPRINA - PRINCÍPIO ATIVO: CLORIDRATO DE CICLOBENZAPRINA; CONCENTRAÇÃO/DOSAGEM: 5MG; FORMA FARMACÊUTICA: COMPRIMIDOS; APRESENTAÇÃO: CAIXA COM 10 COMPRIMIDOS;</t>
   </si>
   <si>
-    <t>GLOBO</t>
-  </si>
-  <si>
     <t>CIMETIDINA - PRINCÍPIO ATIVO: CIMETIDINA; CONCENTRAÇÃO/DOSAGEM: 200MG; FORMA FARMACÊUTICA: COMPRIMIDOS; APRESENTAÇÃO: CAIXA COM 500 COMPRIMIDOS</t>
   </si>
   <si>
@@ -142,9 +112,6 @@
     <t>CLOPIDOGREL - PRINCÍPIO ATIVO:CLOPIDOGREL; CONCENTRAÇÃO DOSAGEM: 75MG; FORMA FAMACÊUTICA: COMPRIMIDOS RESVESTIDOS; APRESENTAÇÃO: CAIXA DE 28 A 56 COMPRIMIDOS</t>
   </si>
   <si>
-    <t>RANBAXY</t>
-  </si>
-  <si>
     <t>CLORETO DE POTÁSSIO - PRINCIPIO ATIVO: CLORETO DE POTÁSSIO; CONCENTRACAO/DOSAGEM: 19,1%; FORMA FARMACEUTICA: SOLUCAO INJETAVEL; APRESENTACAO: AMPOLA 10 ML;</t>
   </si>
   <si>
@@ -154,9 +121,6 @@
     <t>CLORPROMAZINA - PRINCIPIO ATIVO: CLORPROMAZINA, CLORIDRATO; CONCENTRACAO/DOSAGEM: 25 MG; FORMA FARMACEUTICA: COMPRIMIDO.</t>
   </si>
   <si>
-    <t>SANOFI</t>
-  </si>
-  <si>
     <t>CLORPROMAZINA - PRINCÍPIO ATIVO: CLORPROMAZINA; CONCENTRAÇÃO/DOSAGEM: 5MG/ML; FORMA FARMACÊUTICA: SOLUÇÃO INJETÁVEL; APRESNETAÇÃO: AMPOLAS 2ML.</t>
   </si>
   <si>
@@ -178,21 +142,12 @@
     <t>DIAZEPAM - PRINCÍPIO ATIVO: DIAZEPAM; CONCENTRAÇÃO/DOSAGEM: 5MG/ML; FORMA FARMACÊUTICA: SOLUÇÃO INJETÁVEL; APRESENTAÇÃO: AMPOLA 2ML.</t>
   </si>
   <si>
-    <t>CRISTALIA</t>
-  </si>
-  <si>
     <t>DICLOFENACO - PRINCÍPIO ATIVO: DICLOFENACO SÓDICO; CONCENTRAÇÃO DOSAGEM: 25MG/ML; FORMA FARMACÊUTICA: SOLUÇÃO INJETÁVEL; APRESENTAÇÃO: AMPOLAS 3ML.</t>
   </si>
   <si>
-    <t>HYPOFARMA</t>
-  </si>
-  <si>
     <t>DICLOFENACO - PRINCÍPIO ATIVO: DICLOFENACO SÓDICO; CONCENTRAÇÃO DOSAGEM: 50MG; FORMA FARMACÊUTICA: COMPRIMIDOS; APRESENTAÇÃO: CAIXA COM 20 COMPRIMIDOS.</t>
   </si>
   <si>
-    <t>BELFAR</t>
-  </si>
-  <si>
     <t>DIFENIDRAMINA - PRINCÍPIO ATIVO: DIFENIDRAMINA; CONCENTRAÇÃO/DOSAGEM: 50MG/ML; FORMA FARMACÊUTICA: SOLUÇÃO INJETÁVEL; APRESENTAÇÃO: AMPOLAS 1ML.</t>
   </si>
   <si>
@@ -208,15 +163,9 @@
     <t>DIMENIDRINATO + PIRIDOXINA + GLICOSE +FRUTOSE - PRINCÍPIO ATIVO: DIMENIDRINATO + CLORIDRATO DE PIRIDOXINA + GLICOSE + FRUTOSE; CONCENTRAÇÃO/DOSAGEM: 3MG+5MG+100MG/ML + 100MG/ML; FORMA FARMACÊUTICA: SOLUÇÃO INJETÁVEL; APRESENTAÇÃO: AMPOLAS 10ML.</t>
   </si>
   <si>
-    <t>TAKEDA</t>
-  </si>
-  <si>
     <t>DIPIRONA - PRINCÍPIO ATIVO: DIPIRONA; CONCENTRAÇÃO/DOSAGEM: 500MG; FORMA FARMACÊUTICA: COMPRIMIDOS; APRESENTAÇÃO: BLISTER COM 10 COMPRIMIDOS.</t>
   </si>
   <si>
-    <t>VITAMEDIC</t>
-  </si>
-  <si>
     <t>DIPIRONA - PRINCÍPIO ATIVO: DIPIRONA; CONCENTRAÇÃO/DOSAGEM: 500MG; FORMA FARMACÊUTICA: SOLUÇÃO INJETÁVEL; APRESENTAÇÃO: AMPOLAS 2ML.</t>
   </si>
   <si>
@@ -232,9 +181,6 @@
     <t>ENOXAPARINA - PRINCÍPIO ATIVO: ENOXAPARINA; CONCENTRAÇÃO/DOSAGEM: 40MG/0,4ML; FORMA FARMACÊUTICA: SOLUÇÃO INJETÁVEL SC OU IV ; APRESENTAÇÃO: CAIXA COM 10 SERINGAS PREENCHIDAS.</t>
   </si>
   <si>
-    <t>MYLAN</t>
-  </si>
-  <si>
     <t>EPINEFRINA - PRINCÍPIO ATIVO: EPINEFRINA HEMITARTARATO, CONCENTRAÇÃO/DOSAGEM: 1MG/ML; FORMA FARMACÊUTICA: SOLUÇÃO INJETÁVEL; APRESENTAÇÃO: AMPOLA 1ML.</t>
   </si>
   <si>
@@ -274,9 +220,6 @@
     <t>GLICOSE - PRINCIPIO ATIVO: GLICOSE; CONCENTRACAO/DOSAGEM: 250 MG/ML (25%); FORMA FARMACEUTICA: SOLUCAO INJETAVEL; APRESENTACAO: AMPOLA 10 ML.</t>
   </si>
   <si>
-    <t>ISOFARMA</t>
-  </si>
-  <si>
     <t>GLICOSE - PRINCIPIO ATIVO: GLICOSE; CONCENTRACAO/DOSAGEM: 500 MG/ML (50%); FORMA FARMACEUTICA: SOLUCAO INJETAVEL; APRESENTACAO: AMPOLA 10 ML.</t>
   </si>
   <si>
@@ -298,15 +241,9 @@
     <t>IBUPROFENO - PRINCIPIO ATIVO: IBUPROFENO; CONCENTRACAO/DOSAGEM: 100 MG/ML; FORMA FARMACEUTICA: SUSPENSAO ORAL (GOTAS); APRESENTACAO: FRASCO 30 ML.</t>
   </si>
   <si>
-    <t>MEDQUIMICA</t>
-  </si>
-  <si>
     <t>IBUPROFENO - PRINCIPIO ATIVO: IBUPROFENO; CONCENTRACAO/DOSAGEM: 50 MG/ML; FORMA FARMACEUTICA: SUSPENSAO ORAL (GOTAS); APRESENTACAO: FRASCO 30 ML.</t>
   </si>
   <si>
-    <t>NATULAB</t>
-  </si>
-  <si>
     <t>IMIPRAMINA - PRINCÍPIO ATIVO: IMIPRAMINA; CONCENTRAÇÃO/DOSAGEM: 25MG; FORMA FARMACÊUTICA: COMPRIMIDOS; APRESENTAÇÃO: CAIXA COM 30 COMPRIMIDOS.</t>
   </si>
   <si>
@@ -364,15 +301,9 @@
     <t>NOREPINEFRINA - PRINCÍPIO ATIVO: HEMITARTARATO DE NOREPINEFRINA; CONCENTRAÇÃO/DOSAGEM: 2MG/ML; FORMA FARMACÊUTICA: SOLUÇÃO INJETÉVEL INTRAVENOSA; APRESENTAÇÃO: AMPOLAS 4ML.</t>
   </si>
   <si>
-    <t>FRESENIUS</t>
-  </si>
-  <si>
     <t>OLEO MINERAL PURO - PRINCIPIO ATIVO: OLEO MINERAL PURO; CONCENTRACAO/DOSAGEM: 100%; FORMA FARMACEUTICA: OLEO; APRESENTACAO: EMBALAGEM ATE 200 ML.</t>
   </si>
   <si>
-    <t>FARMAX</t>
-  </si>
-  <si>
     <t xml:space="preserve">OMEPRAZOL - PRINCÍPIO ATIVO: OMEPRAZOL; CONCENTRAÇÃO/DOSAGEM: 40MG; FORMA FARMACÊUTICA: PÓ PARA SOLUÇÃO INTRAVENOSA; APRESENTAÇÃO:  FRASCO AMPOLA; COMPONENTE: DILUENTE 10ML.</t>
   </si>
   <si>
@@ -403,18 +334,12 @@
     <t>SALBUTAMOL, SULFATO - PRINCIPIO ATIVO: SALBUTAMOL, SULFATO; CONCENTRACAO/DOSAGEM: 5 MG/ML; FORMA FARMACEUTICA: SOLUCAO PARA NEBULIZACAO; APRESENTACAO: FRASCO 10 ML.</t>
   </si>
   <si>
-    <t>GSK</t>
-  </si>
-  <si>
     <t>SERTRALINA - PRINCÍPIO ATIVO: CLORIDRATO DE SERTRALINA; CONCENTRAÇÃO/DOSAGEM:50MG; FORMA FARMACÊUTICA: COMPRIMIDOS; APRESENTAÇÃO: CAIXA COM 28 OU 30 COMPRIMIDOS.</t>
   </si>
   <si>
     <t>SIMETICONA - PRINCÍPIO ATIVO - SIMETICONA; CONCENTRAÇÃO/DOSAGEM: 40MG; FORMA FARMACÊUTICA: COMPRIMIDOS; APRESENTAÇÃO: CAIXA COM 20 COMPRIMIDOS.</t>
   </si>
   <si>
-    <t>PHARMASCIENCE</t>
-  </si>
-  <si>
     <t>SIMETICONA - PRINCÍPIO ATIVO - SIMETICONA; CONCENTRAÇÃO/DOSAGEM: 75MG/ML; FORMA FARMACÊUTICA: EMULSÃO ORAL; APRESENTAÇÃO: FRASCO 15ML.</t>
   </si>
   <si>
@@ -443,9 +368,6 @@
   </si>
   <si>
     <t>VALSARTANA - PRINCÍPIO ATIVO: VALSARTANA; CONCENTRAÇÃO/DOSAGEM: 160MG; FORMA FARMACÊUTICA: COMPRIMIDOS; APRESENTAÇÃO: CAIXA COM 28 OU 30 COMPRIMIDOS.</t>
-  </si>
-  <si>
-    <t>ALTHAIA</t>
   </si>
   <si>
     <t>VALSARTANA - PRINCÍPIO ATIVO: VALSARTANA; CONCENTRAÇÃO/DOSAGEM: 320MG; FORMA FARMACÊUTICA: COMPRIMIDOS; APRESENTAÇÃO: CAIXA COM 28 OU 30 COMPRIMIDOS.</t>
@@ -854,8 +776,8 @@
       <c r="F2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="2">
-        <v>6.37</v>
+      <c r="G2" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -879,8 +801,8 @@
       <c r="F3" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="2">
-        <v>2.6</v>
+      <c r="G3" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -899,13 +821,13 @@
         <v>400</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="2">
-        <v>3.67</v>
+        <v>8</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -918,7 +840,7 @@
         <v>3143319</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2">
         <v>100</v>
@@ -929,8 +851,8 @@
       <c r="F5" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="2">
-        <v>13</v>
+      <c r="G5" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -943,7 +865,7 @@
         <v>3143320</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2">
         <v>100</v>
@@ -954,8 +876,8 @@
       <c r="F6" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="2">
-        <v>3.25</v>
+      <c r="G6" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -968,19 +890,19 @@
         <v>3143321</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="2">
         <v>600</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="2">
-        <v>34.97</v>
+        <v>8</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -993,19 +915,19 @@
         <v>3143322</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D8" s="2">
         <v>100</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="2">
-        <v>69.42</v>
+        <v>8</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -1018,19 +940,19 @@
         <v>3143323</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D9" s="2">
         <v>1500</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="2">
-        <v>7.35</v>
+        <v>8</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -1043,19 +965,19 @@
         <v>3143324</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D10" s="2">
         <v>1000</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="2">
-        <v>0.25</v>
+        <v>8</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -1068,19 +990,19 @@
         <v>3143325</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D11" s="2">
         <v>100</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="2">
-        <v>2.47</v>
+        <v>8</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -1093,19 +1015,19 @@
         <v>3143326</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D12" s="2">
         <v>600</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="2">
-        <v>19.7</v>
+        <v>8</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -1118,19 +1040,19 @@
         <v>3143327</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D13" s="2">
         <v>200</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="2">
-        <v>3.48</v>
+        <v>8</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -1143,7 +1065,7 @@
         <v>3143328</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D14" s="2">
         <v>100</v>
@@ -1154,8 +1076,8 @@
       <c r="F14" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="2">
-        <v>3.89</v>
+      <c r="G14" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -1168,19 +1090,19 @@
         <v>3143329</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D15" s="2">
         <v>5000</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="G15" s="2">
-        <v>0.3</v>
+        <v>8</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -1193,19 +1115,19 @@
         <v>3143330</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D16" s="2">
         <v>4000</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="2">
-        <v>1.11</v>
+        <v>8</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -1218,19 +1140,19 @@
         <v>3143331</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D17" s="2">
         <v>400</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="G17" s="2">
-        <v>6.24</v>
+        <v>8</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -1243,19 +1165,19 @@
         <v>3143332</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D18" s="2">
         <v>6000</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G18" s="2">
-        <v>0.27</v>
+        <v>8</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -1268,19 +1190,19 @@
         <v>3143333</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D19" s="2">
         <v>1000</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="G19" s="2">
-        <v>0.59</v>
+        <v>8</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -1293,19 +1215,19 @@
         <v>3143334</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D20" s="2">
         <v>12000</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" s="2">
-        <v>0.14</v>
+        <v>8</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -1318,19 +1240,19 @@
         <v>3143335</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D21" s="2">
         <v>600</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" s="2">
-        <v>7.1</v>
+        <v>8</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -1343,19 +1265,19 @@
         <v>3143336</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D22" s="2">
         <v>2000</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22" s="2">
-        <v>0.6</v>
+        <v>8</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -1368,13 +1290,19 @@
         <v>3143337</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D23" s="2">
         <v>100</v>
       </c>
-      <c r="G23" s="2">
-        <v>0</v>
+      <c r="E23" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -1387,13 +1315,19 @@
         <v>3143338</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D24" s="2">
         <v>600</v>
       </c>
-      <c r="G24" s="2">
-        <v>0</v>
+      <c r="E24" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -1406,19 +1340,19 @@
         <v>3143339</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="D25" s="2">
         <v>1000</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="G25" s="2">
-        <v>0.52</v>
+        <v>8</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -1431,7 +1365,7 @@
         <v>3143340</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D26" s="2">
         <v>100</v>
@@ -1442,8 +1376,8 @@
       <c r="F26" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="2">
-        <v>5.2</v>
+      <c r="G26" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -1456,13 +1390,19 @@
         <v>3143341</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D27" s="2">
         <v>20</v>
       </c>
-      <c r="G27" s="2">
-        <v>0</v>
+      <c r="E27" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -1475,13 +1415,19 @@
         <v>3143342</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D28" s="2">
         <v>100</v>
       </c>
-      <c r="G28" s="2">
-        <v>0</v>
+      <c r="E28" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -1494,19 +1440,19 @@
         <v>3143343</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D29" s="2">
         <v>600</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="G29" s="2">
-        <v>3.89</v>
+        <v>8</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -1519,19 +1465,19 @@
         <v>3143344</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D30" s="2">
         <v>800</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="G30" s="2">
-        <v>3.5</v>
+        <v>8</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -1544,19 +1490,19 @@
         <v>3143345</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="D31" s="2">
         <v>1000</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="G31" s="2">
-        <v>7.07</v>
+        <v>8</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -1569,19 +1515,19 @@
         <v>3143346</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D32" s="2">
         <v>200</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="G32" s="2">
-        <v>3.89</v>
+        <v>8</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -1594,19 +1540,19 @@
         <v>3143347</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D33" s="2">
         <v>1000</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="G33" s="2">
-        <v>2.34</v>
+        <v>8</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
@@ -1619,19 +1565,19 @@
         <v>3143348</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D34" s="2">
         <v>10000</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="G34" s="2">
-        <v>0.08</v>
+        <v>8</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -1644,13 +1590,19 @@
         <v>3143349</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="G35" s="2">
-        <v>0</v>
+      <c r="E35" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
@@ -1663,19 +1615,19 @@
         <v>3143350</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="D36" s="2">
         <v>1000</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="G36" s="2">
-        <v>0.26</v>
+        <v>8</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
@@ -1688,19 +1640,19 @@
         <v>3143351</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="D37" s="2">
         <v>1000</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="G37" s="2">
-        <v>0.72</v>
+        <v>8</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
@@ -1713,13 +1665,19 @@
         <v>3143352</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="D38" s="2">
         <v>200</v>
       </c>
-      <c r="G38" s="2">
-        <v>0</v>
+      <c r="E38" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
@@ -1732,19 +1690,19 @@
         <v>3143353</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D39" s="2">
         <v>400</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="G39" s="2">
-        <v>31.2</v>
+        <v>8</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
@@ -1757,19 +1715,19 @@
         <v>3143354</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="D40" s="2">
         <v>30000</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="G40" s="2">
-        <v>0.3</v>
+        <v>8</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
@@ -1782,19 +1740,19 @@
         <v>3143355</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="D41" s="2">
         <v>1000</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="G41" s="2">
-        <v>1.94</v>
+        <v>8</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
@@ -1807,19 +1765,19 @@
         <v>3143356</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="D42" s="2">
         <v>1000</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G42" s="2">
-        <v>3.47</v>
+        <v>8</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
@@ -1832,19 +1790,19 @@
         <v>3143357</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="D43" s="2">
         <v>100</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="G43" s="2">
-        <v>11.7</v>
+        <v>8</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
@@ -1857,13 +1815,19 @@
         <v>3143358</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="D44" s="2">
         <v>100</v>
       </c>
-      <c r="G44" s="2">
-        <v>0</v>
+      <c r="E44" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
@@ -1876,19 +1840,19 @@
         <v>3143359</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="D45" s="2">
         <v>200</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>69</v>
+        <v>8</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="G45" s="2">
-        <v>28.6</v>
+        <v>8</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
@@ -1901,7 +1865,7 @@
         <v>3143360</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="D46" s="2">
         <v>200</v>
@@ -1912,8 +1876,8 @@
       <c r="F46" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G46" s="2">
-        <v>2.73</v>
+      <c r="G46" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
@@ -1926,7 +1890,7 @@
         <v>3143361</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="D47" s="2">
         <v>400</v>
@@ -1937,8 +1901,8 @@
       <c r="F47" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G47" s="2">
-        <v>2.86</v>
+      <c r="G47" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
@@ -1951,19 +1915,19 @@
         <v>3143362</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="D48" s="2">
         <v>8000</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G48" s="2">
-        <v>0.4</v>
+        <v>8</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
@@ -1976,7 +1940,7 @@
         <v>3143363</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="D49" s="2">
         <v>100</v>
@@ -1987,8 +1951,8 @@
       <c r="F49" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G49" s="2">
-        <v>5.19</v>
+      <c r="G49" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
@@ -2001,19 +1965,19 @@
         <v>3143364</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="D50" s="2">
         <v>12000</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="G50" s="2">
-        <v>0.3</v>
+        <v>8</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
@@ -2026,13 +1990,19 @@
         <v>3143365</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="D51" s="2">
         <v>100</v>
       </c>
-      <c r="G51" s="2">
-        <v>0</v>
+      <c r="E51" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
@@ -2045,19 +2015,19 @@
         <v>3143366</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="D52" s="2">
         <v>200</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="G52" s="2">
-        <v>16.9</v>
+        <v>8</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
@@ -2070,19 +2040,19 @@
         <v>3143367</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="D53" s="2">
         <v>100</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G53" s="2">
-        <v>5.42</v>
+        <v>8</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
@@ -2095,19 +2065,19 @@
         <v>3143368</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="D54" s="2">
         <v>1000</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="G54" s="2">
-        <v>10.39</v>
+        <v>8</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
@@ -2120,19 +2090,19 @@
         <v>3143369</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D55" s="2">
         <v>200</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="G55" s="2">
-        <v>2.54</v>
+        <v>8</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
@@ -2145,13 +2115,19 @@
         <v>3143370</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="D56" s="2">
         <v>100</v>
       </c>
-      <c r="G56" s="2">
-        <v>0</v>
+      <c r="E56" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
@@ -2164,19 +2140,19 @@
         <v>3143371</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="D57" s="2">
         <v>5000</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G57" s="2">
-        <v>1.09</v>
+        <v>8</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
@@ -2189,19 +2165,19 @@
         <v>3143372</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="D58" s="2">
         <v>600</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>83</v>
+        <v>8</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="G58" s="2">
-        <v>1.3</v>
+        <v>8</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
@@ -2214,19 +2190,19 @@
         <v>3143373</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D59" s="2">
         <v>600</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>83</v>
+        <v>8</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="G59" s="2">
-        <v>1.3</v>
+        <v>8</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
@@ -2239,13 +2215,19 @@
         <v>3143374</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="D60" s="2">
         <v>100</v>
       </c>
-      <c r="G60" s="2">
-        <v>0</v>
+      <c r="E60" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
@@ -2258,19 +2240,19 @@
         <v>3143375</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="D61" s="2">
         <v>100</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="G61" s="2">
-        <v>8.45</v>
+        <v>8</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
@@ -2283,7 +2265,7 @@
         <v>3143376</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="D62" s="2">
         <v>200</v>
@@ -2294,8 +2276,8 @@
       <c r="F62" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G62" s="2">
-        <v>1.95</v>
+      <c r="G62" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
@@ -2308,13 +2290,19 @@
         <v>3143377</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="D63" s="2">
         <v>20</v>
       </c>
-      <c r="G63" s="2">
-        <v>0</v>
+      <c r="E63" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F63" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
@@ -2327,19 +2315,19 @@
         <v>3143378</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="D64" s="2">
         <v>1000</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="G64" s="2">
-        <v>4.29</v>
+        <v>8</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
@@ -2352,19 +2340,19 @@
         <v>3143379</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="D65" s="2">
         <v>600</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="G65" s="2">
-        <v>6.37</v>
+        <v>8</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
@@ -2377,19 +2365,19 @@
         <v>3143380</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="D66" s="2">
         <v>600</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>93</v>
+        <v>8</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="G66" s="2">
-        <v>3.9</v>
+        <v>8</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
@@ -2402,13 +2390,19 @@
         <v>3143381</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D67" s="2">
         <v>3000</v>
       </c>
-      <c r="G67" s="2">
-        <v>0</v>
+      <c r="E67" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F67" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
@@ -2421,19 +2415,19 @@
         <v>3143382</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="D68" s="2">
         <v>50</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="G68" s="2">
-        <v>21.4</v>
+        <v>8</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
@@ -2446,13 +2440,19 @@
         <v>3143383</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="D69" s="2">
         <v>30</v>
       </c>
-      <c r="G69" s="2">
-        <v>0</v>
+      <c r="E69" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
@@ -2465,19 +2465,19 @@
         <v>3143384</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="D70" s="2">
         <v>200</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="G70" s="2">
-        <v>14.95</v>
+        <v>8</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
@@ -2490,19 +2490,19 @@
         <v>3143385</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="D71" s="2">
         <v>600</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="G71" s="2">
-        <v>11.05</v>
+        <v>8</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
@@ -2515,19 +2515,19 @@
         <v>3143386</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="D72" s="2">
         <v>3000</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G72" s="2">
-        <v>1.01</v>
+        <v>8</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
@@ -2540,13 +2540,19 @@
         <v>3143387</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="D73" s="2">
         <v>200</v>
       </c>
-      <c r="G73" s="2">
-        <v>0</v>
+      <c r="E73" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F73" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
@@ -2559,19 +2565,19 @@
         <v>3143388</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="D74" s="2">
         <v>200</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="G74" s="2">
-        <v>3.12</v>
+        <v>8</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
@@ -2584,19 +2590,19 @@
         <v>3143389</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="D75" s="2">
         <v>400</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>83</v>
+        <v>8</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="G75" s="2">
-        <v>1.42</v>
+        <v>8</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H75" s="2"/>
       <c r="I75" s="2"/>
@@ -2609,19 +2615,19 @@
         <v>3143390</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="D76" s="2">
         <v>50</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="G76" s="2">
-        <v>12.81</v>
+        <v>8</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
@@ -2634,19 +2640,19 @@
         <v>3143391</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="D77" s="2">
         <v>1000</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="G77" s="2">
-        <v>0.31</v>
+        <v>8</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
@@ -2659,19 +2665,19 @@
         <v>3143392</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="D78" s="2">
         <v>200</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="G78" s="2">
-        <v>18.5</v>
+        <v>8</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
@@ -2684,7 +2690,7 @@
         <v>3143393</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="D79" s="2">
         <v>100</v>
@@ -2695,8 +2701,8 @@
       <c r="F79" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G79" s="2">
-        <v>8.97</v>
+      <c r="G79" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H79" s="2"/>
       <c r="I79" s="2"/>
@@ -2709,7 +2715,7 @@
         <v>3143394</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="D80" s="2">
         <v>200</v>
@@ -2720,8 +2726,8 @@
       <c r="F80" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G80" s="2">
-        <v>3.89</v>
+      <c r="G80" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
@@ -2734,19 +2740,19 @@
         <v>3143395</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="D81" s="2">
         <v>800</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="G81" s="2">
-        <v>3.84</v>
+        <v>8</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H81" s="2"/>
       <c r="I81" s="2"/>
@@ -2759,19 +2765,19 @@
         <v>3143396</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="D82" s="2">
         <v>15000</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="G82" s="2">
-        <v>0.17</v>
+        <v>8</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H82" s="2"/>
       <c r="I82" s="2"/>
@@ -2784,19 +2790,19 @@
         <v>3143397</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="D83" s="2">
         <v>100</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="F83" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="G83" s="2">
-        <v>14.37</v>
+        <v>8</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
@@ -2809,13 +2815,19 @@
         <v>3143398</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="D84" s="2">
         <v>2000</v>
       </c>
-      <c r="G84" s="2">
-        <v>0</v>
+      <c r="E84" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F84" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H84" s="2"/>
       <c r="I84" s="2"/>
@@ -2828,19 +2840,19 @@
         <v>3143399</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="D85" s="2">
         <v>200</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>113</v>
+        <v>8</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="G85" s="2">
-        <v>5.19</v>
+        <v>8</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
@@ -2853,19 +2865,19 @@
         <v>3143400</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="D86" s="2">
         <v>200</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>115</v>
+        <v>8</v>
       </c>
       <c r="F86" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="G86" s="2">
-        <v>7.24</v>
+        <v>8</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H86" s="2"/>
       <c r="I86" s="2"/>
@@ -2878,19 +2890,19 @@
         <v>3143401</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="D87" s="2">
         <v>600</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="F87" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="G87" s="2">
-        <v>11.05</v>
+        <v>8</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H87" s="2"/>
       <c r="I87" s="2"/>
@@ -2903,7 +2915,7 @@
         <v>3143402</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="D88" s="2">
         <v>400</v>
@@ -2914,8 +2926,8 @@
       <c r="F88" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G88" s="2">
-        <v>3.64</v>
+      <c r="G88" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
@@ -2928,19 +2940,19 @@
         <v>3143403</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="D89" s="2">
         <v>100</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="F89" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="G89" s="2">
-        <v>8.97</v>
+        <v>8</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
@@ -2953,19 +2965,19 @@
         <v>3143404</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="D90" s="2">
         <v>1000</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>93</v>
+        <v>8</v>
       </c>
       <c r="F90" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="G90" s="2">
-        <v>3.16</v>
+        <v>8</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H90" s="2"/>
       <c r="I90" s="2"/>
@@ -2978,19 +2990,19 @@
         <v>3143405</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="D91" s="2">
         <v>20000</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="F91" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="G91" s="2">
-        <v>0.26</v>
+        <v>8</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H91" s="2"/>
       <c r="I91" s="2"/>
@@ -3003,13 +3015,19 @@
         <v>3143406</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="D92" s="2">
         <v>100</v>
       </c>
-      <c r="G92" s="2">
-        <v>0</v>
+      <c r="E92" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F92" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H92" s="2"/>
       <c r="I92" s="2"/>
@@ -3022,7 +3040,7 @@
         <v>3143407</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="D93" s="2">
         <v>100</v>
@@ -3033,8 +3051,8 @@
       <c r="F93" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G93" s="2">
-        <v>3.9</v>
+      <c r="G93" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H93" s="2"/>
       <c r="I93" s="2"/>
@@ -3047,13 +3065,19 @@
         <v>3143408</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="D94" s="2">
         <v>1000</v>
       </c>
-      <c r="G94" s="2">
-        <v>0</v>
+      <c r="E94" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F94" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H94" s="2"/>
       <c r="I94" s="2"/>
@@ -3066,13 +3090,19 @@
         <v>3143409</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="D95" s="2">
         <v>100</v>
       </c>
-      <c r="G95" s="2">
-        <v>0</v>
+      <c r="E95" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F95" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
@@ -3085,19 +3115,19 @@
         <v>3143410</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="D96" s="2">
         <v>300</v>
       </c>
       <c r="E96" s="0" t="s">
-        <v>126</v>
+        <v>8</v>
       </c>
       <c r="F96" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="G96" s="2">
-        <v>24.19</v>
+        <v>8</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H96" s="2"/>
       <c r="I96" s="2"/>
@@ -3110,19 +3140,19 @@
         <v>3143411</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="D97" s="2">
         <v>12000</v>
       </c>
       <c r="E97" s="0" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="F97" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G97" s="2">
-        <v>0.29</v>
+        <v>8</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H97" s="2"/>
       <c r="I97" s="2"/>
@@ -3135,19 +3165,19 @@
         <v>3143412</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="D98" s="2">
         <v>6000</v>
       </c>
       <c r="E98" s="0" t="s">
-        <v>129</v>
+        <v>8</v>
       </c>
       <c r="F98" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="G98" s="2">
-        <v>0.17</v>
+        <v>8</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H98" s="2"/>
       <c r="I98" s="2"/>
@@ -3160,19 +3190,19 @@
         <v>3143413</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="D99" s="2">
         <v>300</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>93</v>
+        <v>8</v>
       </c>
       <c r="F99" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="G99" s="2">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H99" s="2"/>
       <c r="I99" s="2"/>
@@ -3185,19 +3215,19 @@
         <v>3143414</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="D100" s="2">
         <v>4000</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="F100" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="G100" s="2">
-        <v>0.17</v>
+        <v>8</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H100" s="2"/>
       <c r="I100" s="2"/>
@@ -3210,13 +3240,19 @@
         <v>3143415</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="D101" s="2">
         <v>50</v>
       </c>
-      <c r="G101" s="2">
-        <v>0</v>
+      <c r="E101" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F101" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H101" s="2"/>
       <c r="I101" s="2"/>
@@ -3229,13 +3265,19 @@
         <v>3143416</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="D102" s="2">
         <v>50</v>
       </c>
-      <c r="G102" s="2">
-        <v>0</v>
+      <c r="E102" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F102" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H102" s="2"/>
       <c r="I102" s="2"/>
@@ -3248,13 +3290,19 @@
         <v>3143417</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="D103" s="2">
         <v>50</v>
       </c>
-      <c r="G103" s="2">
-        <v>0</v>
+      <c r="E103" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F103" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H103" s="2"/>
       <c r="I103" s="2"/>
@@ -3267,19 +3315,19 @@
         <v>3143418</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>135</v>
+        <v>110</v>
       </c>
       <c r="D104" s="2">
         <v>200</v>
       </c>
       <c r="E104" s="0" t="s">
-        <v>129</v>
+        <v>8</v>
       </c>
       <c r="F104" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="G104" s="2">
-        <v>4.49</v>
+        <v>8</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H104" s="2"/>
       <c r="I104" s="2"/>
@@ -3292,19 +3340,19 @@
         <v>3143419</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="D105" s="2">
         <v>300</v>
       </c>
       <c r="E105" s="0" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="F105" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="G105" s="2">
-        <v>21.97</v>
+        <v>8</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H105" s="2"/>
       <c r="I105" s="2"/>
@@ -3317,19 +3365,19 @@
         <v>3143420</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="D106" s="2">
         <v>1000</v>
       </c>
       <c r="E106" s="0" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="F106" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="G106" s="2">
-        <v>3.9</v>
+        <v>8</v>
+      </c>
+      <c r="G106" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H106" s="2"/>
       <c r="I106" s="2"/>
@@ -3342,13 +3390,19 @@
         <v>3143421</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="D107" s="2">
         <v>100</v>
       </c>
-      <c r="G107" s="2">
-        <v>0</v>
+      <c r="E107" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F107" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G107" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
@@ -3361,19 +3415,19 @@
         <v>3143422</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="D108" s="2">
         <v>4000</v>
       </c>
       <c r="E108" s="0" t="s">
-        <v>140</v>
+        <v>8</v>
       </c>
       <c r="F108" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="G108" s="2">
-        <v>1.22</v>
+        <v>8</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H108" s="2"/>
       <c r="I108" s="2"/>
@@ -3386,19 +3440,19 @@
         <v>3143423</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="D109" s="2">
         <v>2000</v>
       </c>
       <c r="E109" s="0" t="s">
-        <v>140</v>
+        <v>8</v>
       </c>
       <c r="F109" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="G109" s="2">
-        <v>1.82</v>
+        <v>8</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H109" s="2"/>
       <c r="I109" s="2"/>
@@ -3411,13 +3465,19 @@
         <v>3143424</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="D110" s="2">
         <v>100</v>
       </c>
-      <c r="G110" s="2">
-        <v>0</v>
+      <c r="E110" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F110" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H110" s="2"/>
       <c r="I110" s="2"/>

</xml_diff>

<commit_message>
test: IWorksheet deleted + ModelWorksheetAbs added + LicitanetModel and PcpModel added
</commit_message>
<xml_diff>
--- a/PropProAssistant/Models/LicitaNet/LN_01.xlsx
+++ b/PropProAssistant/Models/LicitaNet/LN_01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Documents\Pregoes_Eletr\DM\Cadastrar\PE_052023_Douradoquara\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DotNETProjects\proppro-assistant\PropProAssistant\Models\LicitaNet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB063C1-9AB5-4ADF-8957-9D2918B87F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF6C64F-A418-4138-A0EB-7513FFFBFEC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,12 @@
   <definedNames>
     <definedName name="TabelaModelo">Worksheet!$A$1:$G$110</definedName>
   </definedNames>
-  <calcPr calcId="999999" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="117">
   <si>
     <t>LOTE</t>
   </si>
@@ -46,7 +46,7 @@
     <t>VALOR UNITÁRIO</t>
   </si>
   <si>
-    <t xml:space="preserve">ÁCIDO TRANEXÂMICO - PRINCÍPIO ATIVO: ÁCIDO TRANEXÊMICO; CONCENTRAÇÃO/DOSAGEM:  50MG/ML; FORMA FARMACÊUTICA: SOLUÇÃO INJETÁVEL; APRESENTAÇÃO: AMPOLAS 5ML.</t>
+    <t>ÁCIDO TRANEXÂMICO - PRINCÍPIO ATIVO: ÁCIDO TRANEXÊMICO; CONCENTRAÇÃO/DOSAGEM:  50MG/ML; FORMA FARMACÊUTICA: SOLUÇÃO INJETÁVEL; APRESENTAÇÃO: AMPOLAS 5ML.</t>
   </si>
   <si>
     <t/>
@@ -196,10 +196,10 @@
     <t>FENOBARBITAL - PRINCIPIO ATIVO: FENOBARBITAL; CONCENTRACAO/DOSAGEM: 100 MG; FORMA FARMACEUTICA: COMPRIMIDO.</t>
   </si>
   <si>
-    <t xml:space="preserve">FENTANILA - PRINCÍPIO ATIVO: FENTANILA. CONCENTRAÇÃO/DOSAGEM: 50MCG/ML; FORMA FARMACÊUTICA:  SOLUÇÃO INJETÁVEL; APRESENTAÇÃO: AMPOLAS 2ML.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FERRO - PRINCÍPIO ATIVO:  SACARATO DE ÓXIDO FÉRRICO; CONCENTRAÇÃO/DOSAGEM: 20MG/ML; FORMA FARMACÊUTICA: SOLUÇÃO INJETÁVEL; APRESENTAÇÃO: CAIXA COM 5 AMPOLAS 5ML.</t>
+    <t>FENTANILA - PRINCÍPIO ATIVO: FENTANILA. CONCENTRAÇÃO/DOSAGEM: 50MCG/ML; FORMA FARMACÊUTICA:  SOLUÇÃO INJETÁVEL; APRESENTAÇÃO: AMPOLAS 2ML.</t>
+  </si>
+  <si>
+    <t>FERRO - PRINCÍPIO ATIVO:  SACARATO DE ÓXIDO FÉRRICO; CONCENTRAÇÃO/DOSAGEM: 20MG/ML; FORMA FARMACÊUTICA: SOLUÇÃO INJETÁVEL; APRESENTAÇÃO: CAIXA COM 5 AMPOLAS 5ML.</t>
   </si>
   <si>
     <t>FLUOCINOLONA ACETONIDA + ASSOCIACOES - PRINCIPIO ATIVO (1): FLUOCINOLONA ACETONIDA; PRINCIPIO ATIVO (2): POLIMIXINA B, SULFATO; PRINCIPIO ATIVO (3): NEOMICINA BASE + LIDOCAINA, CLORIDRATO; CONCENTRACAO/DOSAGEM: 0,250 MG/ML + 10.000 UI/ML + 3,5 MG/ML + 20 MG/ML; FORMA FARMACEUTICA: SOLUCAO OTOLOGICA;</t>
@@ -235,7 +235,7 @@
     <t>HIPROMELOSE - PRINCIPIO ATIVO: HIPROMELOSE; CONCENTRACAO/DOSAGEM: 5 MG/ML; FORMA FARMACEUTICA: SOLUCAO OFTALMICA; APRESENTACAO: FRASCO 10 ML.</t>
   </si>
   <si>
-    <t xml:space="preserve">HYPLEX - PRINCÍPIO ATIVO: COMPLEXO B; FORMA FARMACÊUTICA:  SOLUÇÃO INJETÁVEL; APRESENTAÇÃO: AMPOLAS 2ML.</t>
+    <t>HYPLEX - PRINCÍPIO ATIVO: COMPLEXO B; FORMA FARMACÊUTICA:  SOLUÇÃO INJETÁVEL; APRESENTAÇÃO: AMPOLAS 2ML.</t>
   </si>
   <si>
     <t>IBUPROFENO - PRINCIPIO ATIVO: IBUPROFENO; CONCENTRACAO/DOSAGEM: 100 MG/ML; FORMA FARMACEUTICA: SUSPENSAO ORAL (GOTAS); APRESENTACAO: FRASCO 30 ML.</t>
@@ -304,7 +304,7 @@
     <t>OLEO MINERAL PURO - PRINCIPIO ATIVO: OLEO MINERAL PURO; CONCENTRACAO/DOSAGEM: 100%; FORMA FARMACEUTICA: OLEO; APRESENTACAO: EMBALAGEM ATE 200 ML.</t>
   </si>
   <si>
-    <t xml:space="preserve">OMEPRAZOL - PRINCÍPIO ATIVO: OMEPRAZOL; CONCENTRAÇÃO/DOSAGEM: 40MG; FORMA FARMACÊUTICA: PÓ PARA SOLUÇÃO INTRAVENOSA; APRESENTAÇÃO:  FRASCO AMPOLA; COMPONENTE: DILUENTE 10ML.</t>
+    <t>OMEPRAZOL - PRINCÍPIO ATIVO: OMEPRAZOL; CONCENTRAÇÃO/DOSAGEM: 40MG; FORMA FARMACÊUTICA: PÓ PARA SOLUÇÃO INTRAVENOSA; APRESENTAÇÃO:  FRASCO AMPOLA; COMPONENTE: DILUENTE 10ML.</t>
   </si>
   <si>
     <t>ONDANSETRONA - PRINCÍPIO ATIVO: ONDANSETRONA; CONCENTRAÇÃO/DOSAGEM: 2MG/ML; FORMA FARMACÊUTICA: SOLUÇÃO INJETÁVEL; APRESNETAÇÃO: AMPOLAS 4ML.</t>
@@ -383,7 +383,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -412,10 +412,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -720,23 +720,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I110"/>
+  <dimension ref="A1:G110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="70" customWidth="1" style="1"/>
-    <col min="7" max="9" width="30" customWidth="1"/>
+    <col min="3" max="3" width="70" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -745,23 +745,21 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-    </row>
-    <row r="2" ht="45">
-      <c r="A2" s="0">
+    </row>
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="0">
+      <c r="B2">
         <v>3143316</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -770,23 +768,21 @@
       <c r="D2" s="2">
         <v>200</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="0" t="s">
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
         <v>8</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" ht="45">
-      <c r="A3" s="0">
+    </row>
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3">
         <v>3143317</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -795,23 +791,21 @@
       <c r="D3" s="2">
         <v>200</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="0" t="s">
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
         <v>8</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" ht="45">
-      <c r="A4" s="0">
+    </row>
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="0">
+      <c r="B4">
         <v>3143318</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -820,23 +814,21 @@
       <c r="D4" s="2">
         <v>400</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="0" t="s">
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" ht="45">
-      <c r="A5" s="0">
+    </row>
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="0">
+      <c r="B5">
         <v>3143319</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -845,23 +837,21 @@
       <c r="D5" s="2">
         <v>100</v>
       </c>
-      <c r="E5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="0" t="s">
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
         <v>8</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" ht="45">
-      <c r="A6" s="0">
+    </row>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="0">
+      <c r="B6">
         <v>3143320</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -870,23 +860,21 @@
       <c r="D6" s="2">
         <v>100</v>
       </c>
-      <c r="E6" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="0" t="s">
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
         <v>8</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" ht="60">
-      <c r="A7" s="0">
+    </row>
+    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="0">
+      <c r="B7">
         <v>3143321</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -895,23 +883,21 @@
       <c r="D7" s="2">
         <v>600</v>
       </c>
-      <c r="E7" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="0" t="s">
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
         <v>8</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" ht="60">
-      <c r="A8" s="0">
+    </row>
+    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="0">
+      <c r="B8">
         <v>3143322</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -920,23 +906,21 @@
       <c r="D8" s="2">
         <v>100</v>
       </c>
-      <c r="E8" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="0" t="s">
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" ht="45">
-      <c r="A9" s="0">
-        <v>8</v>
-      </c>
-      <c r="B9" s="0">
+    </row>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
         <v>3143323</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -945,23 +929,21 @@
       <c r="D9" s="2">
         <v>1500</v>
       </c>
-      <c r="E9" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="0" t="s">
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
         <v>8</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" ht="30">
-      <c r="A10" s="0">
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="0">
+      <c r="B10">
         <v>3143324</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -970,23 +952,21 @@
       <c r="D10" s="2">
         <v>1000</v>
       </c>
-      <c r="E10" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="0" t="s">
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
         <v>8</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" ht="45">
-      <c r="A11" s="0">
+    </row>
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="0">
+      <c r="B11">
         <v>3143325</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -995,23 +975,21 @@
       <c r="D11" s="2">
         <v>100</v>
       </c>
-      <c r="E11" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="0" t="s">
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
         <v>8</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" ht="60">
-      <c r="A12" s="0">
+    </row>
+    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="0">
+      <c r="B12">
         <v>3143326</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1020,23 +998,21 @@
       <c r="D12" s="2">
         <v>600</v>
       </c>
-      <c r="E12" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="0" t="s">
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
         <v>8</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" ht="45">
-      <c r="A13" s="0">
+    </row>
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="0">
+      <c r="B13">
         <v>3143327</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1045,23 +1021,21 @@
       <c r="D13" s="2">
         <v>200</v>
       </c>
-      <c r="E13" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="0" t="s">
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
         <v>8</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" ht="45">
-      <c r="A14" s="0">
+    </row>
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="0">
+      <c r="B14">
         <v>3143328</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1070,23 +1044,21 @@
       <c r="D14" s="2">
         <v>100</v>
       </c>
-      <c r="E14" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="0" t="s">
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" t="s">
         <v>8</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" ht="30">
-      <c r="A15" s="0">
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="0">
+      <c r="B15">
         <v>3143329</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1095,23 +1067,21 @@
       <c r="D15" s="2">
         <v>5000</v>
       </c>
-      <c r="E15" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="0" t="s">
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" t="s">
         <v>8</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" ht="30">
-      <c r="A16" s="0">
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="0">
+      <c r="B16">
         <v>3143330</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1120,23 +1090,21 @@
       <c r="D16" s="2">
         <v>4000</v>
       </c>
-      <c r="E16" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="0" t="s">
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" t="s">
         <v>8</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" ht="45">
-      <c r="A17" s="0">
+    </row>
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="0">
+      <c r="B17">
         <v>3143331</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -1145,23 +1113,21 @@
       <c r="D17" s="2">
         <v>400</v>
       </c>
-      <c r="E17" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="0" t="s">
+      <c r="E17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" t="s">
         <v>8</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-    </row>
-    <row r="18" ht="45">
-      <c r="A18" s="0">
+    </row>
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="0">
+      <c r="B18">
         <v>3143332</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -1170,23 +1136,21 @@
       <c r="D18" s="2">
         <v>6000</v>
       </c>
-      <c r="E18" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="0" t="s">
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" t="s">
         <v>8</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-    </row>
-    <row r="19" ht="45">
-      <c r="A19" s="0">
+    </row>
+    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="0">
+      <c r="B19">
         <v>3143333</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -1195,23 +1159,21 @@
       <c r="D19" s="2">
         <v>1000</v>
       </c>
-      <c r="E19" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="0" t="s">
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" t="s">
         <v>8</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" ht="45">
-      <c r="A20" s="0">
+    </row>
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="0">
+      <c r="B20">
         <v>3143334</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -1220,23 +1182,21 @@
       <c r="D20" s="2">
         <v>12000</v>
       </c>
-      <c r="E20" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="0" t="s">
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" t="s">
         <v>8</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-    </row>
-    <row r="21" ht="45">
-      <c r="A21" s="0">
+    </row>
+    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="0">
+      <c r="B21">
         <v>3143335</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -1245,23 +1205,21 @@
       <c r="D21" s="2">
         <v>600</v>
       </c>
-      <c r="E21" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="0" t="s">
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" t="s">
         <v>8</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-    </row>
-    <row r="22" ht="45">
-      <c r="A22" s="0">
+    </row>
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="0">
+      <c r="B22">
         <v>3143336</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -1270,23 +1228,21 @@
       <c r="D22" s="2">
         <v>2000</v>
       </c>
-      <c r="E22" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="0" t="s">
+      <c r="E22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" t="s">
         <v>8</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-    </row>
-    <row r="23" ht="45">
-      <c r="A23" s="0">
+    </row>
+    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="0">
+      <c r="B23">
         <v>3143337</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -1295,23 +1251,21 @@
       <c r="D23" s="2">
         <v>100</v>
       </c>
-      <c r="E23" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="0" t="s">
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" t="s">
         <v>8</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-    </row>
-    <row r="24" ht="45">
-      <c r="A24" s="0">
+    </row>
+    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="0">
+      <c r="B24">
         <v>3143338</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -1320,23 +1274,21 @@
       <c r="D24" s="2">
         <v>600</v>
       </c>
-      <c r="E24" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" s="0" t="s">
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" t="s">
         <v>8</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-    </row>
-    <row r="25" ht="30">
-      <c r="A25" s="0">
+    </row>
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="0">
+      <c r="B25">
         <v>3143339</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -1345,23 +1297,21 @@
       <c r="D25" s="2">
         <v>1000</v>
       </c>
-      <c r="E25" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" s="0" t="s">
+      <c r="E25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" t="s">
         <v>8</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-    </row>
-    <row r="26" ht="45">
-      <c r="A26" s="0">
+    </row>
+    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="0">
+      <c r="B26">
         <v>3143340</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -1370,23 +1320,21 @@
       <c r="D26" s="2">
         <v>100</v>
       </c>
-      <c r="E26" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F26" s="0" t="s">
+      <c r="E26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" t="s">
         <v>8</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-    </row>
-    <row r="27" ht="45">
-      <c r="A27" s="0">
+    </row>
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="0">
+      <c r="B27">
         <v>3143341</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -1395,23 +1343,21 @@
       <c r="D27" s="2">
         <v>20</v>
       </c>
-      <c r="E27" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F27" s="0" t="s">
+      <c r="E27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" t="s">
         <v>8</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-    </row>
-    <row r="28" ht="45">
-      <c r="A28" s="0">
+    </row>
+    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="0">
+      <c r="B28">
         <v>3143342</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -1420,23 +1366,21 @@
       <c r="D28" s="2">
         <v>100</v>
       </c>
-      <c r="E28" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F28" s="0" t="s">
+      <c r="E28" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" t="s">
         <v>8</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-    </row>
-    <row r="29" ht="45">
-      <c r="A29" s="0">
+    </row>
+    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="0">
+      <c r="B29">
         <v>3143343</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -1445,23 +1389,21 @@
       <c r="D29" s="2">
         <v>600</v>
       </c>
-      <c r="E29" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29" s="0" t="s">
+      <c r="E29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" t="s">
         <v>8</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-    </row>
-    <row r="30" ht="45">
-      <c r="A30" s="0">
+    </row>
+    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="0">
+      <c r="B30">
         <v>3143344</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -1470,23 +1412,21 @@
       <c r="D30" s="2">
         <v>800</v>
       </c>
-      <c r="E30" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F30" s="0" t="s">
+      <c r="E30" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" t="s">
         <v>8</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-    </row>
-    <row r="31" ht="45">
-      <c r="A31" s="0">
+    </row>
+    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="0">
+      <c r="B31">
         <v>3143345</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -1495,23 +1435,21 @@
       <c r="D31" s="2">
         <v>1000</v>
       </c>
-      <c r="E31" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F31" s="0" t="s">
+      <c r="E31" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" t="s">
         <v>8</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-    </row>
-    <row r="32" ht="45">
-      <c r="A32" s="0">
+    </row>
+    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="0">
+      <c r="B32">
         <v>3143346</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -1520,23 +1458,21 @@
       <c r="D32" s="2">
         <v>200</v>
       </c>
-      <c r="E32" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F32" s="0" t="s">
+      <c r="E32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" t="s">
         <v>8</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-    </row>
-    <row r="33" ht="45">
-      <c r="A33" s="0">
+    </row>
+    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="0">
+      <c r="B33">
         <v>3143347</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -1545,23 +1481,21 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F33" s="0" t="s">
+      <c r="E33" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" t="s">
         <v>8</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-    </row>
-    <row r="34" ht="45">
-      <c r="A34" s="0">
+    </row>
+    <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="0">
+      <c r="B34">
         <v>3143348</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -1570,23 +1504,21 @@
       <c r="D34" s="2">
         <v>10000</v>
       </c>
-      <c r="E34" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F34" s="0" t="s">
+      <c r="E34" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" t="s">
         <v>8</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-    </row>
-    <row r="35" ht="45">
-      <c r="A35" s="0">
+    </row>
+    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="0">
+      <c r="B35">
         <v>3143349</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -1595,23 +1527,21 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F35" s="0" t="s">
+      <c r="E35" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" t="s">
         <v>8</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-    </row>
-    <row r="36" ht="30">
-      <c r="A36" s="0">
+    </row>
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="0">
+      <c r="B36">
         <v>3143350</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -1620,23 +1550,21 @@
       <c r="D36" s="2">
         <v>1000</v>
       </c>
-      <c r="E36" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F36" s="0" t="s">
+      <c r="E36" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" t="s">
         <v>8</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-    </row>
-    <row r="37" ht="30">
-      <c r="A37" s="0">
+    </row>
+    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="0">
+      <c r="B37">
         <v>3143351</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -1645,23 +1573,21 @@
       <c r="D37" s="2">
         <v>1000</v>
       </c>
-      <c r="E37" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F37" s="0" t="s">
+      <c r="E37" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" t="s">
         <v>8</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-    </row>
-    <row r="38" ht="60">
-      <c r="A38" s="0">
+    </row>
+    <row r="38" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="0">
+      <c r="B38">
         <v>3143352</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -1670,23 +1596,21 @@
       <c r="D38" s="2">
         <v>200</v>
       </c>
-      <c r="E38" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F38" s="0" t="s">
+      <c r="E38" t="s">
+        <v>8</v>
+      </c>
+      <c r="F38" t="s">
         <v>8</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-    </row>
-    <row r="39" ht="60">
-      <c r="A39" s="0">
+    </row>
+    <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="0">
+      <c r="B39">
         <v>3143353</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -1695,23 +1619,21 @@
       <c r="D39" s="2">
         <v>400</v>
       </c>
-      <c r="E39" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F39" s="0" t="s">
+      <c r="E39" t="s">
+        <v>8</v>
+      </c>
+      <c r="F39" t="s">
         <v>8</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-    </row>
-    <row r="40" ht="45">
-      <c r="A40" s="0">
+    </row>
+    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" s="0">
+      <c r="B40">
         <v>3143354</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -1720,23 +1642,21 @@
       <c r="D40" s="2">
         <v>30000</v>
       </c>
-      <c r="E40" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F40" s="0" t="s">
+      <c r="E40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" t="s">
         <v>8</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-    </row>
-    <row r="41" ht="45">
-      <c r="A41" s="0">
+    </row>
+    <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="0">
+      <c r="B41">
         <v>3143355</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -1745,23 +1665,21 @@
       <c r="D41" s="2">
         <v>1000</v>
       </c>
-      <c r="E41" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F41" s="0" t="s">
+      <c r="E41" t="s">
+        <v>8</v>
+      </c>
+      <c r="F41" t="s">
         <v>8</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-    </row>
-    <row r="42" ht="45">
-      <c r="A42" s="0">
+    </row>
+    <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" s="0">
+      <c r="B42">
         <v>3143356</v>
       </c>
       <c r="C42" s="1" t="s">
@@ -1770,23 +1688,21 @@
       <c r="D42" s="2">
         <v>1000</v>
       </c>
-      <c r="E42" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F42" s="0" t="s">
+      <c r="E42" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" t="s">
         <v>8</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-    </row>
-    <row r="43" ht="45">
-      <c r="A43" s="0">
+    </row>
+    <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" s="0">
+      <c r="B43">
         <v>3143357</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -1795,23 +1711,21 @@
       <c r="D43" s="2">
         <v>100</v>
       </c>
-      <c r="E43" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F43" s="0" t="s">
+      <c r="E43" t="s">
+        <v>8</v>
+      </c>
+      <c r="F43" t="s">
         <v>8</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-    </row>
-    <row r="44" ht="45">
-      <c r="A44" s="0">
+    </row>
+    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" s="0">
+      <c r="B44">
         <v>3143358</v>
       </c>
       <c r="C44" s="1" t="s">
@@ -1820,23 +1734,21 @@
       <c r="D44" s="2">
         <v>100</v>
       </c>
-      <c r="E44" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F44" s="0" t="s">
+      <c r="E44" t="s">
+        <v>8</v>
+      </c>
+      <c r="F44" t="s">
         <v>8</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-    </row>
-    <row r="45" ht="60">
-      <c r="A45" s="0">
+    </row>
+    <row r="45" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" s="0">
+      <c r="B45">
         <v>3143359</v>
       </c>
       <c r="C45" s="1" t="s">
@@ -1845,23 +1757,21 @@
       <c r="D45" s="2">
         <v>200</v>
       </c>
-      <c r="E45" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F45" s="0" t="s">
+      <c r="E45" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" t="s">
         <v>8</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-    </row>
-    <row r="46" ht="45">
-      <c r="A46" s="0">
+    </row>
+    <row r="46" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" s="0">
+      <c r="B46">
         <v>3143360</v>
       </c>
       <c r="C46" s="1" t="s">
@@ -1870,23 +1780,21 @@
       <c r="D46" s="2">
         <v>200</v>
       </c>
-      <c r="E46" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F46" s="0" t="s">
+      <c r="E46" t="s">
+        <v>8</v>
+      </c>
+      <c r="F46" t="s">
         <v>8</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-    </row>
-    <row r="47" ht="45">
-      <c r="A47" s="0">
+    </row>
+    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" s="0">
+      <c r="B47">
         <v>3143361</v>
       </c>
       <c r="C47" s="1" t="s">
@@ -1895,23 +1803,21 @@
       <c r="D47" s="2">
         <v>400</v>
       </c>
-      <c r="E47" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F47" s="0" t="s">
+      <c r="E47" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" t="s">
         <v>8</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-    </row>
-    <row r="48" ht="30">
-      <c r="A48" s="0">
+    </row>
+    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" s="0">
+      <c r="B48">
         <v>3143362</v>
       </c>
       <c r="C48" s="1" t="s">
@@ -1920,23 +1826,21 @@
       <c r="D48" s="2">
         <v>8000</v>
       </c>
-      <c r="E48" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F48" s="0" t="s">
+      <c r="E48" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" t="s">
         <v>8</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-    </row>
-    <row r="49" ht="45">
-      <c r="A49" s="0">
+    </row>
+    <row r="49" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" s="0">
+      <c r="B49">
         <v>3143363</v>
       </c>
       <c r="C49" s="1" t="s">
@@ -1945,23 +1849,21 @@
       <c r="D49" s="2">
         <v>100</v>
       </c>
-      <c r="E49" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F49" s="0" t="s">
+      <c r="E49" t="s">
+        <v>8</v>
+      </c>
+      <c r="F49" t="s">
         <v>8</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-    </row>
-    <row r="50" ht="45">
-      <c r="A50" s="0">
+    </row>
+    <row r="50" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50" s="0">
+      <c r="B50">
         <v>3143364</v>
       </c>
       <c r="C50" s="1" t="s">
@@ -1970,23 +1872,21 @@
       <c r="D50" s="2">
         <v>12000</v>
       </c>
-      <c r="E50" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F50" s="0" t="s">
+      <c r="E50" t="s">
+        <v>8</v>
+      </c>
+      <c r="F50" t="s">
         <v>8</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-    </row>
-    <row r="51" ht="45">
-      <c r="A51" s="0">
+    </row>
+    <row r="51" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51" s="0">
+      <c r="B51">
         <v>3143365</v>
       </c>
       <c r="C51" s="1" t="s">
@@ -1995,23 +1895,21 @@
       <c r="D51" s="2">
         <v>100</v>
       </c>
-      <c r="E51" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F51" s="0" t="s">
+      <c r="E51" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" t="s">
         <v>8</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
-    </row>
-    <row r="52" ht="45">
-      <c r="A52" s="0">
+    </row>
+    <row r="52" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52">
         <v>51</v>
       </c>
-      <c r="B52" s="0">
+      <c r="B52">
         <v>3143366</v>
       </c>
       <c r="C52" s="1" t="s">
@@ -2020,23 +1918,21 @@
       <c r="D52" s="2">
         <v>200</v>
       </c>
-      <c r="E52" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F52" s="0" t="s">
+      <c r="E52" t="s">
+        <v>8</v>
+      </c>
+      <c r="F52" t="s">
         <v>8</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-    </row>
-    <row r="53" ht="75">
-      <c r="A53" s="0">
+    </row>
+    <row r="53" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A53">
         <v>52</v>
       </c>
-      <c r="B53" s="0">
+      <c r="B53">
         <v>3143367</v>
       </c>
       <c r="C53" s="1" t="s">
@@ -2045,23 +1941,21 @@
       <c r="D53" s="2">
         <v>100</v>
       </c>
-      <c r="E53" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F53" s="0" t="s">
+      <c r="E53" t="s">
+        <v>8</v>
+      </c>
+      <c r="F53" t="s">
         <v>8</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
-    </row>
-    <row r="54" ht="60">
-      <c r="A54" s="0">
+    </row>
+    <row r="54" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A54">
         <v>53</v>
       </c>
-      <c r="B54" s="0">
+      <c r="B54">
         <v>3143368</v>
       </c>
       <c r="C54" s="1" t="s">
@@ -2070,23 +1964,21 @@
       <c r="D54" s="2">
         <v>1000</v>
       </c>
-      <c r="E54" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F54" s="0" t="s">
+      <c r="E54" t="s">
+        <v>8</v>
+      </c>
+      <c r="F54" t="s">
         <v>8</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
-    </row>
-    <row r="55" ht="45">
-      <c r="A55" s="0">
+    </row>
+    <row r="55" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A55">
         <v>54</v>
       </c>
-      <c r="B55" s="0">
+      <c r="B55">
         <v>3143369</v>
       </c>
       <c r="C55" s="1" t="s">
@@ -2095,23 +1987,21 @@
       <c r="D55" s="2">
         <v>200</v>
       </c>
-      <c r="E55" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F55" s="0" t="s">
+      <c r="E55" t="s">
+        <v>8</v>
+      </c>
+      <c r="F55" t="s">
         <v>8</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-    </row>
-    <row r="56" ht="45">
-      <c r="A56" s="0">
+    </row>
+    <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A56">
         <v>55</v>
       </c>
-      <c r="B56" s="0">
+      <c r="B56">
         <v>3143370</v>
       </c>
       <c r="C56" s="1" t="s">
@@ -2120,23 +2010,21 @@
       <c r="D56" s="2">
         <v>100</v>
       </c>
-      <c r="E56" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F56" s="0" t="s">
+      <c r="E56" t="s">
+        <v>8</v>
+      </c>
+      <c r="F56" t="s">
         <v>8</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2"/>
-    </row>
-    <row r="57" ht="30">
-      <c r="A57" s="0">
+    </row>
+    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57">
         <v>56</v>
       </c>
-      <c r="B57" s="0">
+      <c r="B57">
         <v>3143371</v>
       </c>
       <c r="C57" s="1" t="s">
@@ -2145,23 +2033,21 @@
       <c r="D57" s="2">
         <v>5000</v>
       </c>
-      <c r="E57" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F57" s="0" t="s">
+      <c r="E57" t="s">
+        <v>8</v>
+      </c>
+      <c r="F57" t="s">
         <v>8</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H57" s="2"/>
-      <c r="I57" s="2"/>
-    </row>
-    <row r="58" ht="45">
-      <c r="A58" s="0">
+    </row>
+    <row r="58" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58">
         <v>57</v>
       </c>
-      <c r="B58" s="0">
+      <c r="B58">
         <v>3143372</v>
       </c>
       <c r="C58" s="1" t="s">
@@ -2170,23 +2056,21 @@
       <c r="D58" s="2">
         <v>600</v>
       </c>
-      <c r="E58" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F58" s="0" t="s">
+      <c r="E58" t="s">
+        <v>8</v>
+      </c>
+      <c r="F58" t="s">
         <v>8</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H58" s="2"/>
-      <c r="I58" s="2"/>
-    </row>
-    <row r="59" ht="45">
-      <c r="A59" s="0">
+    </row>
+    <row r="59" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59">
         <v>58</v>
       </c>
-      <c r="B59" s="0">
+      <c r="B59">
         <v>3143373</v>
       </c>
       <c r="C59" s="1" t="s">
@@ -2195,23 +2079,21 @@
       <c r="D59" s="2">
         <v>600</v>
       </c>
-      <c r="E59" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F59" s="0" t="s">
+      <c r="E59" t="s">
+        <v>8</v>
+      </c>
+      <c r="F59" t="s">
         <v>8</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H59" s="2"/>
-      <c r="I59" s="2"/>
-    </row>
-    <row r="60" ht="45">
-      <c r="A60" s="0">
+    </row>
+    <row r="60" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60">
         <v>59</v>
       </c>
-      <c r="B60" s="0">
+      <c r="B60">
         <v>3143374</v>
       </c>
       <c r="C60" s="1" t="s">
@@ -2220,23 +2102,21 @@
       <c r="D60" s="2">
         <v>100</v>
       </c>
-      <c r="E60" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F60" s="0" t="s">
+      <c r="E60" t="s">
+        <v>8</v>
+      </c>
+      <c r="F60" t="s">
         <v>8</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H60" s="2"/>
-      <c r="I60" s="2"/>
-    </row>
-    <row r="61" ht="60">
-      <c r="A61" s="0">
+    </row>
+    <row r="61" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A61">
         <v>60</v>
       </c>
-      <c r="B61" s="0">
+      <c r="B61">
         <v>3143375</v>
       </c>
       <c r="C61" s="1" t="s">
@@ -2245,23 +2125,21 @@
       <c r="D61" s="2">
         <v>100</v>
       </c>
-      <c r="E61" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F61" s="0" t="s">
+      <c r="E61" t="s">
+        <v>8</v>
+      </c>
+      <c r="F61" t="s">
         <v>8</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H61" s="2"/>
-      <c r="I61" s="2"/>
-    </row>
-    <row r="62" ht="45">
-      <c r="A62" s="0">
+    </row>
+    <row r="62" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A62">
         <v>61</v>
       </c>
-      <c r="B62" s="0">
+      <c r="B62">
         <v>3143376</v>
       </c>
       <c r="C62" s="1" t="s">
@@ -2270,23 +2148,21 @@
       <c r="D62" s="2">
         <v>200</v>
       </c>
-      <c r="E62" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F62" s="0" t="s">
+      <c r="E62" t="s">
+        <v>8</v>
+      </c>
+      <c r="F62" t="s">
         <v>8</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H62" s="2"/>
-      <c r="I62" s="2"/>
-    </row>
-    <row r="63" ht="45">
-      <c r="A63" s="0">
+    </row>
+    <row r="63" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A63">
         <v>62</v>
       </c>
-      <c r="B63" s="0">
+      <c r="B63">
         <v>3143377</v>
       </c>
       <c r="C63" s="1" t="s">
@@ -2295,23 +2171,21 @@
       <c r="D63" s="2">
         <v>20</v>
       </c>
-      <c r="E63" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F63" s="0" t="s">
+      <c r="E63" t="s">
+        <v>8</v>
+      </c>
+      <c r="F63" t="s">
         <v>8</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H63" s="2"/>
-      <c r="I63" s="2"/>
-    </row>
-    <row r="64" ht="30">
-      <c r="A64" s="0">
+    </row>
+    <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64">
         <v>63</v>
       </c>
-      <c r="B64" s="0">
+      <c r="B64">
         <v>3143378</v>
       </c>
       <c r="C64" s="1" t="s">
@@ -2320,23 +2194,21 @@
       <c r="D64" s="2">
         <v>1000</v>
       </c>
-      <c r="E64" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F64" s="0" t="s">
+      <c r="E64" t="s">
+        <v>8</v>
+      </c>
+      <c r="F64" t="s">
         <v>8</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
-    </row>
-    <row r="65" ht="45">
-      <c r="A65" s="0">
+    </row>
+    <row r="65" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A65">
         <v>64</v>
       </c>
-      <c r="B65" s="0">
+      <c r="B65">
         <v>3143379</v>
       </c>
       <c r="C65" s="1" t="s">
@@ -2345,23 +2217,21 @@
       <c r="D65" s="2">
         <v>600</v>
       </c>
-      <c r="E65" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F65" s="0" t="s">
+      <c r="E65" t="s">
+        <v>8</v>
+      </c>
+      <c r="F65" t="s">
         <v>8</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H65" s="2"/>
-      <c r="I65" s="2"/>
-    </row>
-    <row r="66" ht="45">
-      <c r="A66" s="0">
+    </row>
+    <row r="66" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A66">
         <v>65</v>
       </c>
-      <c r="B66" s="0">
+      <c r="B66">
         <v>3143380</v>
       </c>
       <c r="C66" s="1" t="s">
@@ -2370,23 +2240,21 @@
       <c r="D66" s="2">
         <v>600</v>
       </c>
-      <c r="E66" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F66" s="0" t="s">
+      <c r="E66" t="s">
+        <v>8</v>
+      </c>
+      <c r="F66" t="s">
         <v>8</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H66" s="2"/>
-      <c r="I66" s="2"/>
-    </row>
-    <row r="67" ht="45">
-      <c r="A67" s="0">
+    </row>
+    <row r="67" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A67">
         <v>66</v>
       </c>
-      <c r="B67" s="0">
+      <c r="B67">
         <v>3143381</v>
       </c>
       <c r="C67" s="1" t="s">
@@ -2395,23 +2263,21 @@
       <c r="D67" s="2">
         <v>3000</v>
       </c>
-      <c r="E67" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F67" s="0" t="s">
+      <c r="E67" t="s">
+        <v>8</v>
+      </c>
+      <c r="F67" t="s">
         <v>8</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H67" s="2"/>
-      <c r="I67" s="2"/>
-    </row>
-    <row r="68" ht="45">
-      <c r="A68" s="0">
+    </row>
+    <row r="68" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A68">
         <v>67</v>
       </c>
-      <c r="B68" s="0">
+      <c r="B68">
         <v>3143382</v>
       </c>
       <c r="C68" s="1" t="s">
@@ -2420,23 +2286,21 @@
       <c r="D68" s="2">
         <v>50</v>
       </c>
-      <c r="E68" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F68" s="0" t="s">
+      <c r="E68" t="s">
+        <v>8</v>
+      </c>
+      <c r="F68" t="s">
         <v>8</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H68" s="2"/>
-      <c r="I68" s="2"/>
-    </row>
-    <row r="69" ht="30">
-      <c r="A69" s="0">
+    </row>
+    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69">
         <v>68</v>
       </c>
-      <c r="B69" s="0">
+      <c r="B69">
         <v>3143383</v>
       </c>
       <c r="C69" s="1" t="s">
@@ -2445,23 +2309,21 @@
       <c r="D69" s="2">
         <v>30</v>
       </c>
-      <c r="E69" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F69" s="0" t="s">
+      <c r="E69" t="s">
+        <v>8</v>
+      </c>
+      <c r="F69" t="s">
         <v>8</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H69" s="2"/>
-      <c r="I69" s="2"/>
-    </row>
-    <row r="70" ht="60">
-      <c r="A70" s="0">
+    </row>
+    <row r="70" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A70">
         <v>69</v>
       </c>
-      <c r="B70" s="0">
+      <c r="B70">
         <v>3143384</v>
       </c>
       <c r="C70" s="1" t="s">
@@ -2470,23 +2332,21 @@
       <c r="D70" s="2">
         <v>200</v>
       </c>
-      <c r="E70" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F70" s="0" t="s">
+      <c r="E70" t="s">
+        <v>8</v>
+      </c>
+      <c r="F70" t="s">
         <v>8</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H70" s="2"/>
-      <c r="I70" s="2"/>
-    </row>
-    <row r="71" ht="45">
-      <c r="A71" s="0">
+    </row>
+    <row r="71" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A71">
         <v>70</v>
       </c>
-      <c r="B71" s="0">
+      <c r="B71">
         <v>3143385</v>
       </c>
       <c r="C71" s="1" t="s">
@@ -2495,23 +2355,21 @@
       <c r="D71" s="2">
         <v>600</v>
       </c>
-      <c r="E71" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F71" s="0" t="s">
+      <c r="E71" t="s">
+        <v>8</v>
+      </c>
+      <c r="F71" t="s">
         <v>8</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H71" s="2"/>
-      <c r="I71" s="2"/>
-    </row>
-    <row r="72" ht="30">
-      <c r="A72" s="0">
+    </row>
+    <row r="72" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72">
         <v>71</v>
       </c>
-      <c r="B72" s="0">
+      <c r="B72">
         <v>3143386</v>
       </c>
       <c r="C72" s="1" t="s">
@@ -2520,23 +2378,21 @@
       <c r="D72" s="2">
         <v>3000</v>
       </c>
-      <c r="E72" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F72" s="0" t="s">
+      <c r="E72" t="s">
+        <v>8</v>
+      </c>
+      <c r="F72" t="s">
         <v>8</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H72" s="2"/>
-      <c r="I72" s="2"/>
-    </row>
-    <row r="73" ht="60">
-      <c r="A73" s="0">
+    </row>
+    <row r="73" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A73">
         <v>72</v>
       </c>
-      <c r="B73" s="0">
+      <c r="B73">
         <v>3143387</v>
       </c>
       <c r="C73" s="1" t="s">
@@ -2545,23 +2401,21 @@
       <c r="D73" s="2">
         <v>200</v>
       </c>
-      <c r="E73" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F73" s="0" t="s">
+      <c r="E73" t="s">
+        <v>8</v>
+      </c>
+      <c r="F73" t="s">
         <v>8</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H73" s="2"/>
-      <c r="I73" s="2"/>
-    </row>
-    <row r="74" ht="45">
-      <c r="A74" s="0">
+    </row>
+    <row r="74" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A74">
         <v>73</v>
       </c>
-      <c r="B74" s="0">
+      <c r="B74">
         <v>3143388</v>
       </c>
       <c r="C74" s="1" t="s">
@@ -2570,23 +2424,21 @@
       <c r="D74" s="2">
         <v>200</v>
       </c>
-      <c r="E74" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F74" s="0" t="s">
+      <c r="E74" t="s">
+        <v>8</v>
+      </c>
+      <c r="F74" t="s">
         <v>8</v>
       </c>
       <c r="G74" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H74" s="2"/>
-      <c r="I74" s="2"/>
-    </row>
-    <row r="75" ht="45">
-      <c r="A75" s="0">
+    </row>
+    <row r="75" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A75">
         <v>74</v>
       </c>
-      <c r="B75" s="0">
+      <c r="B75">
         <v>3143389</v>
       </c>
       <c r="C75" s="1" t="s">
@@ -2595,23 +2447,21 @@
       <c r="D75" s="2">
         <v>400</v>
       </c>
-      <c r="E75" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F75" s="0" t="s">
+      <c r="E75" t="s">
+        <v>8</v>
+      </c>
+      <c r="F75" t="s">
         <v>8</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H75" s="2"/>
-      <c r="I75" s="2"/>
-    </row>
-    <row r="76" ht="45">
-      <c r="A76" s="0">
+    </row>
+    <row r="76" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A76">
         <v>75</v>
       </c>
-      <c r="B76" s="0">
+      <c r="B76">
         <v>3143390</v>
       </c>
       <c r="C76" s="1" t="s">
@@ -2620,23 +2470,21 @@
       <c r="D76" s="2">
         <v>50</v>
       </c>
-      <c r="E76" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F76" s="0" t="s">
+      <c r="E76" t="s">
+        <v>8</v>
+      </c>
+      <c r="F76" t="s">
         <v>8</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H76" s="2"/>
-      <c r="I76" s="2"/>
-    </row>
-    <row r="77" ht="45">
-      <c r="A77" s="0">
+    </row>
+    <row r="77" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A77">
         <v>76</v>
       </c>
-      <c r="B77" s="0">
+      <c r="B77">
         <v>3143391</v>
       </c>
       <c r="C77" s="1" t="s">
@@ -2645,23 +2493,21 @@
       <c r="D77" s="2">
         <v>1000</v>
       </c>
-      <c r="E77" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F77" s="0" t="s">
+      <c r="E77" t="s">
+        <v>8</v>
+      </c>
+      <c r="F77" t="s">
         <v>8</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H77" s="2"/>
-      <c r="I77" s="2"/>
-    </row>
-    <row r="78" ht="45">
-      <c r="A78" s="0">
+    </row>
+    <row r="78" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A78">
         <v>77</v>
       </c>
-      <c r="B78" s="0">
+      <c r="B78">
         <v>3143392</v>
       </c>
       <c r="C78" s="1" t="s">
@@ -2670,23 +2516,21 @@
       <c r="D78" s="2">
         <v>200</v>
       </c>
-      <c r="E78" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F78" s="0" t="s">
+      <c r="E78" t="s">
+        <v>8</v>
+      </c>
+      <c r="F78" t="s">
         <v>8</v>
       </c>
       <c r="G78" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H78" s="2"/>
-      <c r="I78" s="2"/>
-    </row>
-    <row r="79" ht="45">
-      <c r="A79" s="0">
+    </row>
+    <row r="79" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A79">
         <v>78</v>
       </c>
-      <c r="B79" s="0">
+      <c r="B79">
         <v>3143393</v>
       </c>
       <c r="C79" s="1" t="s">
@@ -2695,23 +2539,21 @@
       <c r="D79" s="2">
         <v>100</v>
       </c>
-      <c r="E79" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F79" s="0" t="s">
+      <c r="E79" t="s">
+        <v>8</v>
+      </c>
+      <c r="F79" t="s">
         <v>8</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H79" s="2"/>
-      <c r="I79" s="2"/>
-    </row>
-    <row r="80" ht="45">
-      <c r="A80" s="0">
+    </row>
+    <row r="80" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A80">
         <v>79</v>
       </c>
-      <c r="B80" s="0">
+      <c r="B80">
         <v>3143394</v>
       </c>
       <c r="C80" s="1" t="s">
@@ -2720,23 +2562,21 @@
       <c r="D80" s="2">
         <v>200</v>
       </c>
-      <c r="E80" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F80" s="0" t="s">
+      <c r="E80" t="s">
+        <v>8</v>
+      </c>
+      <c r="F80" t="s">
         <v>8</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H80" s="2"/>
-      <c r="I80" s="2"/>
-    </row>
-    <row r="81" ht="45">
-      <c r="A81" s="0">
+    </row>
+    <row r="81" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A81">
         <v>80</v>
       </c>
-      <c r="B81" s="0">
+      <c r="B81">
         <v>3143395</v>
       </c>
       <c r="C81" s="1" t="s">
@@ -2745,23 +2585,21 @@
       <c r="D81" s="2">
         <v>800</v>
       </c>
-      <c r="E81" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F81" s="0" t="s">
+      <c r="E81" t="s">
+        <v>8</v>
+      </c>
+      <c r="F81" t="s">
         <v>8</v>
       </c>
       <c r="G81" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H81" s="2"/>
-      <c r="I81" s="2"/>
-    </row>
-    <row r="82" ht="45">
-      <c r="A82" s="0">
+    </row>
+    <row r="82" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A82">
         <v>81</v>
       </c>
-      <c r="B82" s="0">
+      <c r="B82">
         <v>3143396</v>
       </c>
       <c r="C82" s="1" t="s">
@@ -2770,23 +2608,21 @@
       <c r="D82" s="2">
         <v>15000</v>
       </c>
-      <c r="E82" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F82" s="0" t="s">
+      <c r="E82" t="s">
+        <v>8</v>
+      </c>
+      <c r="F82" t="s">
         <v>8</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H82" s="2"/>
-      <c r="I82" s="2"/>
-    </row>
-    <row r="83" ht="45">
-      <c r="A83" s="0">
+    </row>
+    <row r="83" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A83">
         <v>82</v>
       </c>
-      <c r="B83" s="0">
+      <c r="B83">
         <v>3143397</v>
       </c>
       <c r="C83" s="1" t="s">
@@ -2795,23 +2631,21 @@
       <c r="D83" s="2">
         <v>100</v>
       </c>
-      <c r="E83" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F83" s="0" t="s">
+      <c r="E83" t="s">
+        <v>8</v>
+      </c>
+      <c r="F83" t="s">
         <v>8</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H83" s="2"/>
-      <c r="I83" s="2"/>
-    </row>
-    <row r="84" ht="45">
-      <c r="A84" s="0">
+    </row>
+    <row r="84" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A84">
         <v>83</v>
       </c>
-      <c r="B84" s="0">
+      <c r="B84">
         <v>3143398</v>
       </c>
       <c r="C84" s="1" t="s">
@@ -2820,23 +2654,21 @@
       <c r="D84" s="2">
         <v>2000</v>
       </c>
-      <c r="E84" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F84" s="0" t="s">
+      <c r="E84" t="s">
+        <v>8</v>
+      </c>
+      <c r="F84" t="s">
         <v>8</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H84" s="2"/>
-      <c r="I84" s="2"/>
-    </row>
-    <row r="85" ht="45">
-      <c r="A85" s="0">
+    </row>
+    <row r="85" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A85">
         <v>84</v>
       </c>
-      <c r="B85" s="0">
+      <c r="B85">
         <v>3143399</v>
       </c>
       <c r="C85" s="1" t="s">
@@ -2845,23 +2677,21 @@
       <c r="D85" s="2">
         <v>200</v>
       </c>
-      <c r="E85" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F85" s="0" t="s">
+      <c r="E85" t="s">
+        <v>8</v>
+      </c>
+      <c r="F85" t="s">
         <v>8</v>
       </c>
       <c r="G85" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H85" s="2"/>
-      <c r="I85" s="2"/>
-    </row>
-    <row r="86" ht="45">
-      <c r="A86" s="0">
+    </row>
+    <row r="86" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A86">
         <v>85</v>
       </c>
-      <c r="B86" s="0">
+      <c r="B86">
         <v>3143400</v>
       </c>
       <c r="C86" s="1" t="s">
@@ -2870,23 +2700,21 @@
       <c r="D86" s="2">
         <v>200</v>
       </c>
-      <c r="E86" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F86" s="0" t="s">
+      <c r="E86" t="s">
+        <v>8</v>
+      </c>
+      <c r="F86" t="s">
         <v>8</v>
       </c>
       <c r="G86" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H86" s="2"/>
-      <c r="I86" s="2"/>
-    </row>
-    <row r="87" ht="45">
-      <c r="A87" s="0">
+    </row>
+    <row r="87" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A87">
         <v>86</v>
       </c>
-      <c r="B87" s="0">
+      <c r="B87">
         <v>3143401</v>
       </c>
       <c r="C87" s="1" t="s">
@@ -2895,23 +2723,21 @@
       <c r="D87" s="2">
         <v>600</v>
       </c>
-      <c r="E87" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F87" s="0" t="s">
+      <c r="E87" t="s">
+        <v>8</v>
+      </c>
+      <c r="F87" t="s">
         <v>8</v>
       </c>
       <c r="G87" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H87" s="2"/>
-      <c r="I87" s="2"/>
-    </row>
-    <row r="88" ht="45">
-      <c r="A88" s="0">
+    </row>
+    <row r="88" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A88">
         <v>87</v>
       </c>
-      <c r="B88" s="0">
+      <c r="B88">
         <v>3143402</v>
       </c>
       <c r="C88" s="1" t="s">
@@ -2920,23 +2746,21 @@
       <c r="D88" s="2">
         <v>400</v>
       </c>
-      <c r="E88" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F88" s="0" t="s">
+      <c r="E88" t="s">
+        <v>8</v>
+      </c>
+      <c r="F88" t="s">
         <v>8</v>
       </c>
       <c r="G88" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H88" s="2"/>
-      <c r="I88" s="2"/>
-    </row>
-    <row r="89" ht="45">
-      <c r="A89" s="0">
+    </row>
+    <row r="89" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A89">
         <v>88</v>
       </c>
-      <c r="B89" s="0">
+      <c r="B89">
         <v>3143403</v>
       </c>
       <c r="C89" s="1" t="s">
@@ -2945,23 +2769,21 @@
       <c r="D89" s="2">
         <v>100</v>
       </c>
-      <c r="E89" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F89" s="0" t="s">
+      <c r="E89" t="s">
+        <v>8</v>
+      </c>
+      <c r="F89" t="s">
         <v>8</v>
       </c>
       <c r="G89" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H89" s="2"/>
-      <c r="I89" s="2"/>
-    </row>
-    <row r="90" ht="45">
-      <c r="A90" s="0">
+    </row>
+    <row r="90" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A90">
         <v>89</v>
       </c>
-      <c r="B90" s="0">
+      <c r="B90">
         <v>3143404</v>
       </c>
       <c r="C90" s="1" t="s">
@@ -2970,23 +2792,21 @@
       <c r="D90" s="2">
         <v>1000</v>
       </c>
-      <c r="E90" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F90" s="0" t="s">
+      <c r="E90" t="s">
+        <v>8</v>
+      </c>
+      <c r="F90" t="s">
         <v>8</v>
       </c>
       <c r="G90" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H90" s="2"/>
-      <c r="I90" s="2"/>
-    </row>
-    <row r="91" ht="45">
-      <c r="A91" s="0">
+    </row>
+    <row r="91" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A91">
         <v>90</v>
       </c>
-      <c r="B91" s="0">
+      <c r="B91">
         <v>3143405</v>
       </c>
       <c r="C91" s="1" t="s">
@@ -2995,23 +2815,21 @@
       <c r="D91" s="2">
         <v>20000</v>
       </c>
-      <c r="E91" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F91" s="0" t="s">
+      <c r="E91" t="s">
+        <v>8</v>
+      </c>
+      <c r="F91" t="s">
         <v>8</v>
       </c>
       <c r="G91" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H91" s="2"/>
-      <c r="I91" s="2"/>
-    </row>
-    <row r="92" ht="45">
-      <c r="A92" s="0">
+    </row>
+    <row r="92" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A92">
         <v>91</v>
       </c>
-      <c r="B92" s="0">
+      <c r="B92">
         <v>3143406</v>
       </c>
       <c r="C92" s="1" t="s">
@@ -3020,23 +2838,21 @@
       <c r="D92" s="2">
         <v>100</v>
       </c>
-      <c r="E92" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F92" s="0" t="s">
+      <c r="E92" t="s">
+        <v>8</v>
+      </c>
+      <c r="F92" t="s">
         <v>8</v>
       </c>
       <c r="G92" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H92" s="2"/>
-      <c r="I92" s="2"/>
-    </row>
-    <row r="93" ht="45">
-      <c r="A93" s="0">
+    </row>
+    <row r="93" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A93">
         <v>92</v>
       </c>
-      <c r="B93" s="0">
+      <c r="B93">
         <v>3143407</v>
       </c>
       <c r="C93" s="1" t="s">
@@ -3045,23 +2861,21 @@
       <c r="D93" s="2">
         <v>100</v>
       </c>
-      <c r="E93" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F93" s="0" t="s">
+      <c r="E93" t="s">
+        <v>8</v>
+      </c>
+      <c r="F93" t="s">
         <v>8</v>
       </c>
       <c r="G93" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H93" s="2"/>
-      <c r="I93" s="2"/>
-    </row>
-    <row r="94" ht="45">
-      <c r="A94" s="0">
+    </row>
+    <row r="94" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A94">
         <v>93</v>
       </c>
-      <c r="B94" s="0">
+      <c r="B94">
         <v>3143408</v>
       </c>
       <c r="C94" s="1" t="s">
@@ -3070,23 +2884,21 @@
       <c r="D94" s="2">
         <v>1000</v>
       </c>
-      <c r="E94" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F94" s="0" t="s">
+      <c r="E94" t="s">
+        <v>8</v>
+      </c>
+      <c r="F94" t="s">
         <v>8</v>
       </c>
       <c r="G94" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H94" s="2"/>
-      <c r="I94" s="2"/>
-    </row>
-    <row r="95" ht="45">
-      <c r="A95" s="0">
+    </row>
+    <row r="95" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A95">
         <v>94</v>
       </c>
-      <c r="B95" s="0">
+      <c r="B95">
         <v>3143409</v>
       </c>
       <c r="C95" s="1" t="s">
@@ -3095,23 +2907,21 @@
       <c r="D95" s="2">
         <v>100</v>
       </c>
-      <c r="E95" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F95" s="0" t="s">
+      <c r="E95" t="s">
+        <v>8</v>
+      </c>
+      <c r="F95" t="s">
         <v>8</v>
       </c>
       <c r="G95" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H95" s="2"/>
-      <c r="I95" s="2"/>
-    </row>
-    <row r="96" ht="45">
-      <c r="A96" s="0">
+    </row>
+    <row r="96" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A96">
         <v>95</v>
       </c>
-      <c r="B96" s="0">
+      <c r="B96">
         <v>3143410</v>
       </c>
       <c r="C96" s="1" t="s">
@@ -3120,23 +2930,21 @@
       <c r="D96" s="2">
         <v>300</v>
       </c>
-      <c r="E96" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F96" s="0" t="s">
+      <c r="E96" t="s">
+        <v>8</v>
+      </c>
+      <c r="F96" t="s">
         <v>8</v>
       </c>
       <c r="G96" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H96" s="2"/>
-      <c r="I96" s="2"/>
-    </row>
-    <row r="97" ht="45">
-      <c r="A97" s="0">
+    </row>
+    <row r="97" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A97">
         <v>96</v>
       </c>
-      <c r="B97" s="0">
+      <c r="B97">
         <v>3143411</v>
       </c>
       <c r="C97" s="1" t="s">
@@ -3145,23 +2953,21 @@
       <c r="D97" s="2">
         <v>12000</v>
       </c>
-      <c r="E97" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F97" s="0" t="s">
+      <c r="E97" t="s">
+        <v>8</v>
+      </c>
+      <c r="F97" t="s">
         <v>8</v>
       </c>
       <c r="G97" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H97" s="2"/>
-      <c r="I97" s="2"/>
-    </row>
-    <row r="98" ht="45">
-      <c r="A98" s="0">
+    </row>
+    <row r="98" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A98">
         <v>97</v>
       </c>
-      <c r="B98" s="0">
+      <c r="B98">
         <v>3143412</v>
       </c>
       <c r="C98" s="1" t="s">
@@ -3170,23 +2976,21 @@
       <c r="D98" s="2">
         <v>6000</v>
       </c>
-      <c r="E98" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F98" s="0" t="s">
+      <c r="E98" t="s">
+        <v>8</v>
+      </c>
+      <c r="F98" t="s">
         <v>8</v>
       </c>
       <c r="G98" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H98" s="2"/>
-      <c r="I98" s="2"/>
-    </row>
-    <row r="99" ht="45">
-      <c r="A99" s="0">
+    </row>
+    <row r="99" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A99">
         <v>98</v>
       </c>
-      <c r="B99" s="0">
+      <c r="B99">
         <v>3143413</v>
       </c>
       <c r="C99" s="1" t="s">
@@ -3195,23 +2999,21 @@
       <c r="D99" s="2">
         <v>300</v>
       </c>
-      <c r="E99" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F99" s="0" t="s">
+      <c r="E99" t="s">
+        <v>8</v>
+      </c>
+      <c r="F99" t="s">
         <v>8</v>
       </c>
       <c r="G99" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H99" s="2"/>
-      <c r="I99" s="2"/>
-    </row>
-    <row r="100" ht="30">
-      <c r="A100" s="0">
+    </row>
+    <row r="100" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A100">
         <v>99</v>
       </c>
-      <c r="B100" s="0">
+      <c r="B100">
         <v>3143414</v>
       </c>
       <c r="C100" s="1" t="s">
@@ -3220,23 +3022,21 @@
       <c r="D100" s="2">
         <v>4000</v>
       </c>
-      <c r="E100" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F100" s="0" t="s">
+      <c r="E100" t="s">
+        <v>8</v>
+      </c>
+      <c r="F100" t="s">
         <v>8</v>
       </c>
       <c r="G100" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H100" s="2"/>
-      <c r="I100" s="2"/>
-    </row>
-    <row r="101" ht="45">
-      <c r="A101" s="0">
+    </row>
+    <row r="101" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A101">
         <v>100</v>
       </c>
-      <c r="B101" s="0">
+      <c r="B101">
         <v>3143415</v>
       </c>
       <c r="C101" s="1" t="s">
@@ -3245,23 +3045,21 @@
       <c r="D101" s="2">
         <v>50</v>
       </c>
-      <c r="E101" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F101" s="0" t="s">
+      <c r="E101" t="s">
+        <v>8</v>
+      </c>
+      <c r="F101" t="s">
         <v>8</v>
       </c>
       <c r="G101" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H101" s="2"/>
-      <c r="I101" s="2"/>
-    </row>
-    <row r="102" ht="60">
-      <c r="A102" s="0">
+    </row>
+    <row r="102" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A102">
         <v>101</v>
       </c>
-      <c r="B102" s="0">
+      <c r="B102">
         <v>3143416</v>
       </c>
       <c r="C102" s="1" t="s">
@@ -3270,23 +3068,21 @@
       <c r="D102" s="2">
         <v>50</v>
       </c>
-      <c r="E102" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F102" s="0" t="s">
+      <c r="E102" t="s">
+        <v>8</v>
+      </c>
+      <c r="F102" t="s">
         <v>8</v>
       </c>
       <c r="G102" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H102" s="2"/>
-      <c r="I102" s="2"/>
-    </row>
-    <row r="103" ht="45">
-      <c r="A103" s="0">
+    </row>
+    <row r="103" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A103">
         <v>102</v>
       </c>
-      <c r="B103" s="0">
+      <c r="B103">
         <v>3143417</v>
       </c>
       <c r="C103" s="1" t="s">
@@ -3295,23 +3091,21 @@
       <c r="D103" s="2">
         <v>50</v>
       </c>
-      <c r="E103" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F103" s="0" t="s">
+      <c r="E103" t="s">
+        <v>8</v>
+      </c>
+      <c r="F103" t="s">
         <v>8</v>
       </c>
       <c r="G103" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H103" s="2"/>
-      <c r="I103" s="2"/>
-    </row>
-    <row r="104" ht="45">
-      <c r="A104" s="0">
+    </row>
+    <row r="104" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A104">
         <v>103</v>
       </c>
-      <c r="B104" s="0">
+      <c r="B104">
         <v>3143418</v>
       </c>
       <c r="C104" s="1" t="s">
@@ -3320,23 +3114,21 @@
       <c r="D104" s="2">
         <v>200</v>
       </c>
-      <c r="E104" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F104" s="0" t="s">
+      <c r="E104" t="s">
+        <v>8</v>
+      </c>
+      <c r="F104" t="s">
         <v>8</v>
       </c>
       <c r="G104" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H104" s="2"/>
-      <c r="I104" s="2"/>
-    </row>
-    <row r="105" ht="45">
-      <c r="A105" s="0">
+    </row>
+    <row r="105" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A105">
         <v>104</v>
       </c>
-      <c r="B105" s="0">
+      <c r="B105">
         <v>3143419</v>
       </c>
       <c r="C105" s="1" t="s">
@@ -3345,23 +3137,21 @@
       <c r="D105" s="2">
         <v>300</v>
       </c>
-      <c r="E105" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F105" s="0" t="s">
+      <c r="E105" t="s">
+        <v>8</v>
+      </c>
+      <c r="F105" t="s">
         <v>8</v>
       </c>
       <c r="G105" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H105" s="2"/>
-      <c r="I105" s="2"/>
-    </row>
-    <row r="106" ht="45">
-      <c r="A106" s="0">
+    </row>
+    <row r="106" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A106">
         <v>105</v>
       </c>
-      <c r="B106" s="0">
+      <c r="B106">
         <v>3143420</v>
       </c>
       <c r="C106" s="1" t="s">
@@ -3370,23 +3160,21 @@
       <c r="D106" s="2">
         <v>1000</v>
       </c>
-      <c r="E106" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F106" s="0" t="s">
+      <c r="E106" t="s">
+        <v>8</v>
+      </c>
+      <c r="F106" t="s">
         <v>8</v>
       </c>
       <c r="G106" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H106" s="2"/>
-      <c r="I106" s="2"/>
-    </row>
-    <row r="107" ht="60">
-      <c r="A107" s="0">
+    </row>
+    <row r="107" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A107">
         <v>106</v>
       </c>
-      <c r="B107" s="0">
+      <c r="B107">
         <v>3143421</v>
       </c>
       <c r="C107" s="1" t="s">
@@ -3395,23 +3183,21 @@
       <c r="D107" s="2">
         <v>100</v>
       </c>
-      <c r="E107" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F107" s="0" t="s">
+      <c r="E107" t="s">
+        <v>8</v>
+      </c>
+      <c r="F107" t="s">
         <v>8</v>
       </c>
       <c r="G107" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H107" s="2"/>
-      <c r="I107" s="2"/>
-    </row>
-    <row r="108" ht="45">
-      <c r="A108" s="0">
+    </row>
+    <row r="108" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A108">
         <v>107</v>
       </c>
-      <c r="B108" s="0">
+      <c r="B108">
         <v>3143422</v>
       </c>
       <c r="C108" s="1" t="s">
@@ -3420,23 +3206,21 @@
       <c r="D108" s="2">
         <v>4000</v>
       </c>
-      <c r="E108" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F108" s="0" t="s">
+      <c r="E108" t="s">
+        <v>8</v>
+      </c>
+      <c r="F108" t="s">
         <v>8</v>
       </c>
       <c r="G108" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H108" s="2"/>
-      <c r="I108" s="2"/>
-    </row>
-    <row r="109" ht="45">
-      <c r="A109" s="0">
+    </row>
+    <row r="109" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A109">
         <v>108</v>
       </c>
-      <c r="B109" s="0">
+      <c r="B109">
         <v>3143423</v>
       </c>
       <c r="C109" s="1" t="s">
@@ -3445,23 +3229,21 @@
       <c r="D109" s="2">
         <v>2000</v>
       </c>
-      <c r="E109" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F109" s="0" t="s">
+      <c r="E109" t="s">
+        <v>8</v>
+      </c>
+      <c r="F109" t="s">
         <v>8</v>
       </c>
       <c r="G109" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H109" s="2"/>
-      <c r="I109" s="2"/>
-    </row>
-    <row r="110" ht="45">
-      <c r="A110" s="0">
+    </row>
+    <row r="110" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A110">
         <v>109</v>
       </c>
-      <c r="B110" s="0">
+      <c r="B110">
         <v>3143424</v>
       </c>
       <c r="C110" s="1" t="s">
@@ -3470,21 +3252,18 @@
       <c r="D110" s="2">
         <v>100</v>
       </c>
-      <c r="E110" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F110" s="0" t="s">
+      <c r="E110" t="s">
+        <v>8</v>
+      </c>
+      <c r="F110" t="s">
         <v>8</v>
       </c>
       <c r="G110" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H110" s="2"/>
-      <c r="I110" s="2"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>